<commit_message>
Improve Grov analysis and add JSON output for volatility
Enhanced Grov analysis by refining rise event logic and adding a new JSON output for volatility analysis. Removed unused debug and test scripts.

- Deleted `debug_grov.py` and `test_grov_logic.py` as they are no longer needed
- Updated `analyze_grov_rise_events.py` with improved rise event detection logic
- Modified `GrovPocView.jsx` to reflect updated analysis output
- Added `grov_rise_volatility_analysis.json` for detailed volatility insights
- Updated `grov_rise_events.xlsx` with new analysis data
- Adjusted process IDs in `node-server.pid` and `vite.pid` logs

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/grov_rise_events.xlsx
+++ b/output CSVs/grov_rise_events.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,33 +505,29 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>13/06/2022</t>
+          <t>26/08/2021</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>17/06/2022</t>
+          <t>06/06/2022</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5</v>
+        <v>196</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>68.06999999999999</v>
+        <v>3.21</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>4/49</t>
+          <t>38/39</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>68.06999999999999</v>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>16/06/2022</t>
-        </is>
-      </c>
+        <v>3.21</v>
+      </c>
+      <c r="H2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -541,29 +537,33 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>17/06/2022</t>
+          <t>06/06/2022</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>18/07/2022</t>
+          <t>20/07/2022</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>-55</v>
+        <v>-55.02</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>46/48</t>
+          <t>36/38</t>
         </is>
       </c>
       <c r="G3" s="3" t="n">
-        <v>13.07</v>
-      </c>
-      <c r="H3" s="3" t="inlineStr"/>
+        <v>-51.81</v>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>16/06/2022</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -573,7 +573,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>18/07/2022</t>
+          <t>20/07/2022</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -582,18 +582,18 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2.44</v>
+        <v>2.9</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>49/49</t>
+          <t>39/39</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>15.51</v>
+        <v>-48.91</v>
       </c>
       <c r="H4" s="2" t="inlineStr"/>
     </row>
@@ -621,11 +621,11 @@
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>15/48</t>
+          <t>7/38</t>
         </is>
       </c>
       <c r="G5" s="3" t="n">
-        <v>5.1</v>
+        <v>-59.32</v>
       </c>
       <c r="H5" s="3" t="inlineStr"/>
     </row>
@@ -653,11 +653,11 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>3/49</t>
+          <t>3/39</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>74.11</v>
+        <v>9.69</v>
       </c>
       <c r="H6" s="2" t="inlineStr"/>
     </row>
@@ -674,24 +674,28 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>26/08/2022</t>
+          <t>30/08/2022</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>-31.38</v>
+        <v>-32.66</v>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>41/48</t>
+          <t>30/38</t>
         </is>
       </c>
       <c r="G7" s="3" t="n">
-        <v>42.73</v>
-      </c>
-      <c r="H7" s="3" t="inlineStr"/>
+        <v>-22.98</v>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>30/08/2022</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -701,7 +705,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>26/08/2022</t>
+          <t>30/08/2022</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
@@ -710,18 +714,18 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45.09</v>
+        <v>47.87</v>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>8/49</t>
+          <t>7/39</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
-        <v>87.81999999999999</v>
+        <v>24.89</v>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
@@ -753,11 +757,11 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>47/48</t>
+          <t>37/38</t>
         </is>
       </c>
       <c r="G9" s="3" t="n">
-        <v>8.4</v>
+        <v>-54.53</v>
       </c>
       <c r="H9" s="3" t="inlineStr"/>
     </row>
@@ -785,11 +789,11 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>31/49</t>
+          <t>28/39</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>20.29</v>
+        <v>-42.64</v>
       </c>
       <c r="H10" s="2" t="inlineStr"/>
     </row>
@@ -817,11 +821,11 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>42/48</t>
+          <t>31/38</t>
         </is>
       </c>
       <c r="G11" s="3" t="n">
-        <v>-12.84</v>
+        <v>-75.77</v>
       </c>
       <c r="H11" s="3" t="inlineStr"/>
     </row>
@@ -849,11 +853,11 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>19/49</t>
+          <t>20/39</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
-        <v>4.92</v>
+        <v>-58.01</v>
       </c>
       <c r="H12" s="2" t="inlineStr"/>
     </row>
@@ -881,11 +885,11 @@
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>48/48</t>
+          <t>38/38</t>
         </is>
       </c>
       <c r="G13" s="3" t="n">
-        <v>-78.81</v>
+        <v>-141.74</v>
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
@@ -917,11 +921,11 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>1/49</t>
+          <t>1/39</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
-        <v>118.75</v>
+        <v>55.82</v>
       </c>
       <c r="H14" s="2" t="inlineStr"/>
     </row>
@@ -938,22 +942,22 @@
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>26/01/2023</t>
+          <t>30/01/2023</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>-26.39</v>
+        <v>-29.51</v>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>38/48</t>
+          <t>27/38</t>
         </is>
       </c>
       <c r="G15" s="3" t="n">
-        <v>92.36</v>
+        <v>26.32</v>
       </c>
       <c r="H15" s="3" t="inlineStr"/>
     </row>
@@ -965,27 +969,27 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>26/01/2023</t>
+          <t>30/01/2023</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>06/02/2023</t>
+          <t>08/02/2023</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
         <v>8</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>16.7</v>
+        <v>17.21</v>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>21/49</t>
+          <t>22/39</t>
         </is>
       </c>
       <c r="G16" s="2" t="n">
-        <v>109.06</v>
+        <v>43.53</v>
       </c>
       <c r="H16" s="2" t="inlineStr"/>
     </row>
@@ -997,7 +1001,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>06/02/2023</t>
+          <t>08/02/2023</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -1006,18 +1010,18 @@
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>-23.47</v>
+        <v>-20.44</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>33/48</t>
+          <t>22/38</t>
         </is>
       </c>
       <c r="G17" s="3" t="n">
-        <v>85.59</v>
+        <v>23.09</v>
       </c>
       <c r="H17" s="3" t="inlineStr"/>
     </row>
@@ -1045,11 +1049,11 @@
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>10/49</t>
+          <t>9/39</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>125.24</v>
+        <v>62.74</v>
       </c>
       <c r="H18" s="2" t="inlineStr"/>
     </row>
@@ -1077,11 +1081,11 @@
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>44/48</t>
+          <t>34/38</t>
         </is>
       </c>
       <c r="G19" s="3" t="n">
-        <v>84.16</v>
+        <v>21.67</v>
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
@@ -1113,11 +1117,11 @@
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>6/49</t>
+          <t>5/39</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
-        <v>136.58</v>
+        <v>74.09</v>
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
@@ -1149,11 +1153,11 @@
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>19/48</t>
+          <t>8/38</t>
         </is>
       </c>
       <c r="G21" s="3" t="n">
-        <v>124.86</v>
+        <v>62.36</v>
       </c>
       <c r="H21" s="3" t="inlineStr"/>
     </row>
@@ -1170,22 +1174,22 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>18/04/2023</t>
+          <t>28/04/2023</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>13.06</v>
+        <v>10.36</v>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>28/49</t>
+          <t>29/39</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
-        <v>137.92</v>
+        <v>72.72</v>
       </c>
       <c r="H22" s="2" t="inlineStr"/>
     </row>
@@ -1197,7 +1201,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>18/04/2023</t>
+          <t>28/04/2023</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1206,18 +1210,18 @@
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>-10.76</v>
+        <v>-8.57</v>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>16/48</t>
+          <t>5/38</t>
         </is>
       </c>
       <c r="G23" s="3" t="n">
-        <v>127.16</v>
+        <v>64.15000000000001</v>
       </c>
       <c r="H23" s="3" t="inlineStr"/>
     </row>
@@ -1245,11 +1249,11 @@
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>17/49</t>
+          <t>17/39</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
-        <v>147.7</v>
+        <v>84.69</v>
       </c>
       <c r="H24" s="2" t="inlineStr">
         <is>
@@ -1270,22 +1274,22 @@
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>09/06/2023</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>-39.26</v>
+        <v>-33.7</v>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>43/48</t>
+          <t>32/38</t>
         </is>
       </c>
       <c r="G25" s="3" t="n">
-        <v>108.44</v>
+        <v>50.98</v>
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
@@ -1301,29 +1305,33 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>09/06/2023</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>16/06/2023</t>
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>33.54</v>
+        <v>13.41</v>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>13/49</t>
+          <t>27/39</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>141.98</v>
-      </c>
-      <c r="H26" s="2" t="inlineStr"/>
+        <v>64.39</v>
+      </c>
+      <c r="H26" s="2" t="inlineStr">
+        <is>
+          <t>09/06/2023</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
@@ -1333,27 +1341,27 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>16/06/2023</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>27/07/2023</t>
+          <t>27/06/2023</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>-12.33</v>
+        <v>-19.21</v>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>20/48</t>
+          <t>18/38</t>
         </is>
       </c>
       <c r="G27" s="3" t="n">
-        <v>129.65</v>
+        <v>45.18</v>
       </c>
       <c r="H27" s="3" t="inlineStr"/>
     </row>
@@ -1365,27 +1373,27 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>27/07/2023</t>
+          <t>27/06/2023</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>29/08/2023</t>
+          <t>12/07/2023</t>
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>86.98</v>
+        <v>33.54</v>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>2/49</t>
+          <t>12/39</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>216.63</v>
+        <v>78.72</v>
       </c>
       <c r="H28" s="2" t="inlineStr"/>
     </row>
@@ -1397,27 +1405,27 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>29/08/2023</t>
+          <t>12/07/2023</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>21/09/2023</t>
+          <t>31/07/2023</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>-26.74</v>
+        <v>-15.53</v>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>39/48</t>
+          <t>14/38</t>
         </is>
       </c>
       <c r="G29" s="3" t="n">
-        <v>189.89</v>
+        <v>63.2</v>
       </c>
       <c r="H29" s="3" t="inlineStr"/>
     </row>
@@ -1429,27 +1437,27 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>21/09/2023</t>
+          <t>31/07/2023</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>26/09/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>6.08</v>
+        <v>94.05</v>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>43/49</t>
+          <t>2/39</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>195.97</v>
+        <v>157.25</v>
       </c>
       <c r="H30" s="2" t="inlineStr"/>
     </row>
@@ -1461,27 +1469,27 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>26/09/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>13/10/2023</t>
+          <t>21/09/2023</t>
         </is>
       </c>
       <c r="D31" s="3" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>-41.94</v>
+        <v>-26.74</v>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>45/48</t>
+          <t>25/38</t>
         </is>
       </c>
       <c r="G31" s="3" t="n">
-        <v>154.03</v>
+        <v>130.5</v>
       </c>
       <c r="H31" s="3" t="inlineStr"/>
     </row>
@@ -1493,27 +1501,27 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>13/10/2023</t>
+          <t>21/09/2023</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>19/10/2023</t>
+          <t>26/09/2023</t>
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>16.67</v>
+        <v>6.08</v>
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>22/49</t>
+          <t>36/39</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
-        <v>170.7</v>
+        <v>136.58</v>
       </c>
       <c r="H32" s="2" t="inlineStr"/>
     </row>
@@ -1525,27 +1533,27 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>19/10/2023</t>
+          <t>26/09/2023</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>01/11/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="D33" s="3" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>-19.58</v>
+        <v>-41.94</v>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>27/48</t>
+          <t>35/38</t>
         </is>
       </c>
       <c r="G33" s="3" t="n">
-        <v>151.13</v>
+        <v>94.65000000000001</v>
       </c>
       <c r="H33" s="3" t="inlineStr"/>
     </row>
@@ -1557,27 +1565,27 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>01/11/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>22/11/2023</t>
+          <t>19/10/2023</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>53.95</v>
+        <v>16.67</v>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>5/49</t>
+          <t>23/39</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>205.08</v>
+        <v>111.32</v>
       </c>
       <c r="H34" s="2" t="inlineStr"/>
     </row>
@@ -1589,33 +1597,29 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>22/11/2023</t>
+          <t>19/10/2023</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="D35" s="3" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E35" s="3" t="n">
-        <v>-22.22</v>
+        <v>-19.58</v>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>32/48</t>
+          <t>19/38</t>
         </is>
       </c>
       <c r="G35" s="3" t="n">
-        <v>182.85</v>
-      </c>
-      <c r="H35" s="3" t="inlineStr">
-        <is>
-          <t>14/12/2023</t>
-        </is>
-      </c>
+        <v>91.73999999999999</v>
+      </c>
+      <c r="H35" s="3" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
@@ -1625,27 +1629,27 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>01/11/2023</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>22/11/2023</t>
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>16.48</v>
+        <v>53.95</v>
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>23/49</t>
+          <t>4/39</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>199.33</v>
+        <v>145.69</v>
       </c>
       <c r="H36" s="2" t="inlineStr"/>
     </row>
@@ -1657,29 +1661,33 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>22/11/2023</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>26/01/2024</t>
+          <t>20/12/2023</t>
         </is>
       </c>
       <c r="D37" s="3" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>-19.81</v>
+        <v>-22.22</v>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>30/48</t>
+          <t>23/38</t>
         </is>
       </c>
       <c r="G37" s="3" t="n">
-        <v>179.52</v>
-      </c>
-      <c r="H37" s="3" t="inlineStr"/>
+        <v>123.47</v>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>14/12/2023</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
@@ -1689,27 +1697,27 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>26/01/2024</t>
+          <t>20/12/2023</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>31/01/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>7.65</v>
+        <v>16.48</v>
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>41/49</t>
+          <t>24/39</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>187.17</v>
+        <v>139.95</v>
       </c>
       <c r="H38" s="2" t="inlineStr"/>
     </row>
@@ -1721,27 +1729,27 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>31/01/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>20/02/2024</t>
+          <t>26/01/2024</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
         <v>13</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>-9.289999999999999</v>
+        <v>-19.81</v>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>12/48</t>
+          <t>20/38</t>
         </is>
       </c>
       <c r="G39" s="3" t="n">
-        <v>177.88</v>
+        <v>120.14</v>
       </c>
       <c r="H39" s="3" t="inlineStr"/>
     </row>
@@ -1753,27 +1761,27 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>20/02/2024</t>
+          <t>26/01/2024</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>05/03/2024</t>
+          <t>31/01/2024</t>
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>38.55</v>
+        <v>7.65</v>
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>11/49</t>
+          <t>33/39</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>216.43</v>
+        <v>127.79</v>
       </c>
       <c r="H40" s="2" t="inlineStr"/>
     </row>
@@ -1785,33 +1793,29 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>05/03/2024</t>
+          <t>31/01/2024</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>12/03/2024</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>-25.22</v>
+        <v>-9.84</v>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>36/48</t>
+          <t>6/38</t>
         </is>
       </c>
       <c r="G41" s="3" t="n">
-        <v>191.22</v>
-      </c>
-      <c r="H41" s="3" t="inlineStr">
-        <is>
-          <t>08/03/2024, 11/03/2024</t>
-        </is>
-      </c>
+        <v>117.95</v>
+      </c>
+      <c r="H41" s="3" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
@@ -1821,27 +1825,27 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>12/03/2024</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>15/03/2024</t>
+          <t>05/03/2024</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>12.21</v>
+        <v>39.39</v>
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>30/49</t>
+          <t>10/39</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>203.43</v>
+        <v>157.34</v>
       </c>
       <c r="H42" s="2" t="inlineStr"/>
     </row>
@@ -1853,7 +1857,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>15/03/2024</t>
+          <t>05/03/2024</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -1862,20 +1866,24 @@
         </is>
       </c>
       <c r="D43" s="3" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>-19.69</v>
+        <v>-32.61</v>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>28/48</t>
+          <t>29/38</t>
         </is>
       </c>
       <c r="G43" s="3" t="n">
-        <v>183.74</v>
-      </c>
-      <c r="H43" s="3" t="inlineStr"/>
+        <v>124.73</v>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>08/03/2024, 11/03/2024</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
@@ -1901,11 +1909,11 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>36/49</t>
+          <t>31/39</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>193.42</v>
+        <v>134.41</v>
       </c>
       <c r="H44" s="2" t="inlineStr"/>
     </row>
@@ -1933,11 +1941,11 @@
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>23/48</t>
+          <t>13/38</t>
         </is>
       </c>
       <c r="G45" s="3" t="n">
-        <v>178.12</v>
+        <v>119.12</v>
       </c>
       <c r="H45" s="3" t="inlineStr"/>
     </row>
@@ -1965,11 +1973,11 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>18/49</t>
+          <t>19/39</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
-        <v>196.87</v>
+        <v>137.87</v>
       </c>
       <c r="H46" s="2" t="inlineStr"/>
     </row>
@@ -1997,11 +2005,11 @@
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>21/48</t>
+          <t>11/38</t>
         </is>
       </c>
       <c r="G47" s="3" t="n">
-        <v>182.84</v>
+        <v>123.83</v>
       </c>
       <c r="H47" s="3" t="inlineStr"/>
     </row>
@@ -2029,11 +2037,11 @@
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>35/49</t>
+          <t>30/39</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>193.04</v>
+        <v>134.03</v>
       </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
@@ -2065,11 +2073,11 @@
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>5/48</t>
+          <t>3/38</t>
         </is>
       </c>
       <c r="G49" s="3" t="n">
-        <v>187.48</v>
+        <v>128.48</v>
       </c>
       <c r="H49" s="3" t="inlineStr"/>
     </row>
@@ -2086,22 +2094,22 @@
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>14/06/2024</t>
+          <t>03/07/2024</t>
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>15.03</v>
+        <v>20.26</v>
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>24/49</t>
+          <t>18/39</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>202.51</v>
+        <v>148.74</v>
       </c>
       <c r="H50" s="2" t="inlineStr"/>
     </row>
@@ -2113,27 +2121,27 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>14/06/2024</t>
+          <t>03/07/2024</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>18/06/2024</t>
+          <t>28/08/2024</t>
         </is>
       </c>
       <c r="D51" s="3" t="n">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>-8.52</v>
+        <v>-30.98</v>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>11/48</t>
+          <t>28/38</t>
         </is>
       </c>
       <c r="G51" s="3" t="n">
-        <v>193.99</v>
+        <v>117.76</v>
       </c>
       <c r="H51" s="3" t="inlineStr"/>
     </row>
@@ -2145,27 +2153,27 @@
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>18/06/2024</t>
+          <t>28/08/2024</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>03/07/2024</t>
+          <t>19/09/2024</t>
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>14.29</v>
+        <v>14.17</v>
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>26/49</t>
+          <t>26/39</t>
         </is>
       </c>
       <c r="G52" s="2" t="n">
-        <v>208.28</v>
+        <v>131.93</v>
       </c>
       <c r="H52" s="2" t="inlineStr"/>
     </row>
@@ -2177,27 +2185,27 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>03/07/2024</t>
+          <t>19/09/2024</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>30/07/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="D53" s="3" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>-25</v>
+        <v>-12.41</v>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>35/48</t>
+          <t>9/38</t>
         </is>
       </c>
       <c r="G53" s="3" t="n">
-        <v>183.28</v>
+        <v>119.52</v>
       </c>
       <c r="H53" s="3" t="inlineStr"/>
     </row>
@@ -2209,27 +2217,27 @@
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>30/07/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>02/08/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>10.87</v>
+        <v>14.96</v>
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>34/49</t>
+          <t>25/39</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
-        <v>194.15</v>
+        <v>134.48</v>
       </c>
       <c r="H54" s="2" t="inlineStr"/>
     </row>
@@ -2241,27 +2249,27 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>02/08/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>28/08/2024</t>
+          <t>30/10/2024</t>
         </is>
       </c>
       <c r="D55" s="3" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>-16.99</v>
+        <v>-13.7</v>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>26/48</t>
+          <t>10/38</t>
         </is>
       </c>
       <c r="G55" s="3" t="n">
-        <v>177.16</v>
+        <v>120.78</v>
       </c>
       <c r="H55" s="3" t="inlineStr"/>
     </row>
@@ -2273,27 +2281,27 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>28/08/2024</t>
+          <t>30/10/2024</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>12/11/2024</t>
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>14.17</v>
+        <v>20.63</v>
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>27/49</t>
+          <t>16/39</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
-        <v>191.33</v>
+        <v>141.41</v>
       </c>
       <c r="H56" s="2" t="inlineStr"/>
     </row>
@@ -2305,27 +2313,27 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>12/11/2024</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>15/11/2024</t>
         </is>
       </c>
       <c r="D57" s="3" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>-11.72</v>
+        <v>-15.13</v>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>18/48</t>
+          <t>12/38</t>
         </is>
       </c>
       <c r="G57" s="3" t="n">
-        <v>179.6</v>
+        <v>126.28</v>
       </c>
       <c r="H57" s="3" t="inlineStr"/>
     </row>
@@ -2337,29 +2345,33 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>15/11/2024</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>08/01/2025</t>
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>3.13</v>
+        <v>36.43</v>
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>47/49</t>
+          <t>11/39</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
-        <v>182.73</v>
-      </c>
-      <c r="H58" s="2" t="inlineStr"/>
+        <v>162.71</v>
+      </c>
+      <c r="H58" s="2" t="inlineStr">
+        <is>
+          <t>18/11/2024</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
@@ -2369,27 +2381,27 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>08/01/2025</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>15/01/2025</t>
         </is>
       </c>
       <c r="D59" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>-3.79</v>
+        <v>-26.14</v>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>1/48</t>
+          <t>24/38</t>
         </is>
       </c>
       <c r="G59" s="3" t="n">
-        <v>178.94</v>
+        <v>136.57</v>
       </c>
       <c r="H59" s="3" t="inlineStr"/>
     </row>
@@ -2401,27 +2413,27 @@
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>15/01/2025</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>05/02/2025</t>
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>14.96</v>
+        <v>31.54</v>
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>25/49</t>
+          <t>14/39</t>
         </is>
       </c>
       <c r="G60" s="2" t="n">
-        <v>193.9</v>
+        <v>168.11</v>
       </c>
       <c r="H60" s="2" t="inlineStr"/>
     </row>
@@ -2433,27 +2445,27 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>05/02/2025</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>07/02/2025</t>
         </is>
       </c>
       <c r="D61" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>-6.85</v>
+        <v>-8.19</v>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>8/48</t>
+          <t>4/38</t>
         </is>
       </c>
       <c r="G61" s="3" t="n">
-        <v>187.05</v>
+        <v>159.92</v>
       </c>
       <c r="H61" s="3" t="inlineStr"/>
     </row>
@@ -2465,27 +2477,27 @@
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>07/02/2025</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/03/2025</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>11.76</v>
+        <v>6.37</v>
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>32/49</t>
+          <t>35/39</t>
         </is>
       </c>
       <c r="G62" s="2" t="n">
-        <v>198.81</v>
+        <v>166.29</v>
       </c>
       <c r="H62" s="2" t="inlineStr"/>
     </row>
@@ -2497,27 +2509,27 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/03/2025</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>15/11/2024</t>
+          <t>11/04/2025</t>
         </is>
       </c>
       <c r="D63" s="3" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>-15.13</v>
+        <v>-37.13</v>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>22/48</t>
+          <t>33/38</t>
         </is>
       </c>
       <c r="G63" s="3" t="n">
-        <v>183.68</v>
+        <v>129.17</v>
       </c>
       <c r="H63" s="3" t="inlineStr"/>
     </row>
@@ -2529,33 +2541,29 @@
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>15/11/2024</t>
+          <t>11/04/2025</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>22/11/2024</t>
+          <t>29/04/2025</t>
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>7.75</v>
+        <v>8.57</v>
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>39/49</t>
+          <t>32/39</t>
         </is>
       </c>
       <c r="G64" s="2" t="n">
-        <v>191.43</v>
-      </c>
-      <c r="H64" s="2" t="inlineStr">
-        <is>
-          <t>18/11/2024</t>
-        </is>
-      </c>
+        <v>137.74</v>
+      </c>
+      <c r="H64" s="2" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
@@ -2565,27 +2573,27 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>22/11/2024</t>
+          <t>29/04/2025</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>26/11/2024</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="D65" s="3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>-5.76</v>
+        <v>-5.26</v>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>6/48</t>
+          <t>2/38</t>
         </is>
       </c>
       <c r="G65" s="3" t="n">
-        <v>185.68</v>
+        <v>132.47</v>
       </c>
       <c r="H65" s="3" t="inlineStr"/>
     </row>
@@ -2597,29 +2605,33 @@
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>26/11/2024</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>08/01/2025</t>
+          <t>27/05/2025</t>
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>34.35</v>
+        <v>32.41</v>
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>12/49</t>
+          <t>13/39</t>
         </is>
       </c>
       <c r="G66" s="2" t="n">
-        <v>220.03</v>
-      </c>
-      <c r="H66" s="2" t="inlineStr"/>
+        <v>164.88</v>
+      </c>
+      <c r="H66" s="2" t="inlineStr">
+        <is>
+          <t>20/05/2025, 21/05/2025, 22/05/2025, 23/05/2025, 27/05/2025</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
@@ -2629,29 +2641,33 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>08/01/2025</t>
+          <t>27/05/2025</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>15/01/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="D67" s="3" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>-26.14</v>
+        <v>-27.97</v>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>37/48</t>
+          <t>26/38</t>
         </is>
       </c>
       <c r="G67" s="3" t="n">
-        <v>193.89</v>
-      </c>
-      <c r="H67" s="3" t="inlineStr"/>
+        <v>136.91</v>
+      </c>
+      <c r="H67" s="3" t="inlineStr">
+        <is>
+          <t>02/06/2025, 06/06/2025, 09/06/2025, 10/06/2025, 12/06/2025, 13/06/2025, 27/05/2025, 28/05/2025, 29/05/2025</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
@@ -2661,27 +2677,27 @@
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>15/01/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>23/01/2025</t>
+          <t>11/07/2025</t>
         </is>
       </c>
       <c r="D68" s="2" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>11.54</v>
+        <v>48.54</v>
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>33/49</t>
+          <t>6/39</t>
         </is>
       </c>
       <c r="G68" s="2" t="n">
-        <v>205.43</v>
+        <v>185.45</v>
       </c>
       <c r="H68" s="2" t="inlineStr"/>
     </row>
@@ -2693,27 +2709,27 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>23/01/2025</t>
+          <t>11/07/2025</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>27/01/2025</t>
+          <t>07/08/2025</t>
         </is>
       </c>
       <c r="D69" s="3" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>-6.9</v>
+        <v>-15.69</v>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>9/48</t>
+          <t>15/38</t>
         </is>
       </c>
       <c r="G69" s="3" t="n">
-        <v>198.54</v>
+        <v>169.77</v>
       </c>
       <c r="H69" s="3" t="inlineStr"/>
     </row>
@@ -2725,27 +2741,27 @@
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>27/01/2025</t>
+          <t>07/08/2025</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>05/02/2025</t>
+          <t>15/08/2025</t>
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>26.67</v>
+        <v>21.71</v>
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>15/49</t>
+          <t>15/39</t>
         </is>
       </c>
       <c r="G70" s="2" t="n">
-        <v>225.21</v>
+        <v>191.48</v>
       </c>
       <c r="H70" s="2" t="inlineStr"/>
     </row>
@@ -2757,27 +2773,27 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>05/02/2025</t>
+          <t>15/08/2025</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>07/10/2025</t>
         </is>
       </c>
       <c r="D71" s="3" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>-8.19</v>
+        <v>-4.46</v>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>10/48</t>
+          <t>1/38</t>
         </is>
       </c>
       <c r="G71" s="3" t="n">
-        <v>217.02</v>
+        <v>187.02</v>
       </c>
       <c r="H71" s="3" t="inlineStr"/>
     </row>
@@ -2789,27 +2805,27 @@
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>07/10/2025</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>12/02/2025</t>
+          <t>17/10/2025</t>
         </is>
       </c>
       <c r="D72" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E72" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E72" s="2" t="n">
-        <v>8.279999999999999</v>
-      </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>38/49</t>
+          <t>37/39</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
-        <v>225.3</v>
+        <v>191.02</v>
       </c>
       <c r="H72" s="2" t="inlineStr"/>
     </row>
@@ -2821,27 +2837,27 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>12/02/2025</t>
+          <t>17/10/2025</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t>04/03/2025</t>
+          <t>04/11/2025</t>
         </is>
       </c>
       <c r="D73" s="3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E73" s="3" t="n">
-        <v>-4.71</v>
+        <v>-19.87</v>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>3/48</t>
+          <t>21/38</t>
         </is>
       </c>
       <c r="G73" s="3" t="n">
-        <v>220.59</v>
+        <v>171.15</v>
       </c>
       <c r="H73" s="3" t="inlineStr"/>
     </row>
@@ -2853,27 +2869,27 @@
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>04/03/2025</t>
+          <t>04/11/2025</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>13/03/2025</t>
+          <t>14/11/2025</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>3.09</v>
+        <v>17.6</v>
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>48/49</t>
+          <t>21/39</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
-        <v>223.68</v>
+        <v>188.75</v>
       </c>
       <c r="H74" s="2" t="inlineStr"/>
     </row>
@@ -2885,27 +2901,27 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>13/03/2025</t>
+          <t>14/11/2025</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>28/03/2025</t>
+          <t>08/12/2025</t>
         </is>
       </c>
       <c r="D75" s="3" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E75" s="3" t="n">
-        <v>-19.76</v>
+        <v>-16.33</v>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>29/48</t>
+          <t>16/38</t>
         </is>
       </c>
       <c r="G75" s="3" t="n">
-        <v>203.92</v>
+        <v>172.42</v>
       </c>
       <c r="H75" s="3" t="inlineStr"/>
     </row>
@@ -2917,27 +2933,27 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>28/03/2025</t>
+          <t>08/12/2025</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>03/04/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>3.73</v>
+        <v>7.32</v>
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>46/49</t>
+          <t>34/39</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
-        <v>207.65</v>
+        <v>179.74</v>
       </c>
       <c r="H76" s="2" t="inlineStr"/>
     </row>
@@ -2949,27 +2965,27 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>03/04/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>11/04/2025</t>
+          <t>31/12/2025</t>
         </is>
       </c>
       <c r="D77" s="3" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>-24.46</v>
+        <v>-16.67</v>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>34/48</t>
+          <t>17/38</t>
         </is>
       </c>
       <c r="G77" s="3" t="n">
-        <v>183.19</v>
+        <v>163.07</v>
       </c>
       <c r="H77" s="3" t="inlineStr"/>
     </row>
@@ -2981,677 +2997,29 @@
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>11/04/2025</t>
+          <t>31/12/2025</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>17/02/2026</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>8.57</v>
+        <v>40</v>
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>37/49</t>
+          <t>8/39</t>
         </is>
       </c>
       <c r="G78" s="2" t="n">
-        <v>191.76</v>
+        <v>203.07</v>
       </c>
       <c r="H78" s="2" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B79" s="3" t="inlineStr">
-        <is>
-          <t>29/04/2025</t>
-        </is>
-      </c>
-      <c r="C79" s="3" t="inlineStr">
-        <is>
-          <t>06/05/2025</t>
-        </is>
-      </c>
-      <c r="D79" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E79" s="3" t="n">
-        <v>-5.26</v>
-      </c>
-      <c r="F79" s="3" t="inlineStr">
-        <is>
-          <t>4/48</t>
-        </is>
-      </c>
-      <c r="G79" s="3" t="n">
-        <v>186.5</v>
-      </c>
-      <c r="H79" s="3" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B80" s="2" t="inlineStr">
-        <is>
-          <t>06/05/2025</t>
-        </is>
-      </c>
-      <c r="C80" s="2" t="inlineStr">
-        <is>
-          <t>12/05/2025</t>
-        </is>
-      </c>
-      <c r="D80" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E80" s="2" t="n">
-        <v>12.96</v>
-      </c>
-      <c r="F80" s="2" t="inlineStr">
-        <is>
-          <t>29/49</t>
-        </is>
-      </c>
-      <c r="G80" s="2" t="n">
-        <v>199.46</v>
-      </c>
-      <c r="H80" s="2" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B81" s="3" t="inlineStr">
-        <is>
-          <t>12/05/2025</t>
-        </is>
-      </c>
-      <c r="C81" s="3" t="inlineStr">
-        <is>
-          <t>19/05/2025</t>
-        </is>
-      </c>
-      <c r="D81" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E81" s="3" t="n">
-        <v>-9.84</v>
-      </c>
-      <c r="F81" s="3" t="inlineStr">
-        <is>
-          <t>13/48</t>
-        </is>
-      </c>
-      <c r="G81" s="3" t="n">
-        <v>189.62</v>
-      </c>
-      <c r="H81" s="3" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B82" s="2" t="inlineStr">
-        <is>
-          <t>19/05/2025</t>
-        </is>
-      </c>
-      <c r="C82" s="2" t="inlineStr">
-        <is>
-          <t>27/05/2025</t>
-        </is>
-      </c>
-      <c r="D82" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E82" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="F82" s="2" t="inlineStr">
-        <is>
-          <t>14/49</t>
-        </is>
-      </c>
-      <c r="G82" s="2" t="n">
-        <v>219.62</v>
-      </c>
-      <c r="H82" s="2" t="inlineStr">
-        <is>
-          <t>20/05/2025, 21/05/2025, 22/05/2025, 23/05/2025, 27/05/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B83" s="3" t="inlineStr">
-        <is>
-          <t>27/05/2025</t>
-        </is>
-      </c>
-      <c r="C83" s="3" t="inlineStr">
-        <is>
-          <t>20/06/2025</t>
-        </is>
-      </c>
-      <c r="D83" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="E83" s="3" t="n">
-        <v>-27.97</v>
-      </c>
-      <c r="F83" s="3" t="inlineStr">
-        <is>
-          <t>40/48</t>
-        </is>
-      </c>
-      <c r="G83" s="3" t="n">
-        <v>191.65</v>
-      </c>
-      <c r="H83" s="3" t="inlineStr">
-        <is>
-          <t>02/06/2025, 06/06/2025, 09/06/2025, 10/06/2025, 12/06/2025, 13/06/2025, 27/05/2025, 28/05/2025, 29/05/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B84" s="2" t="inlineStr">
-        <is>
-          <t>20/06/2025</t>
-        </is>
-      </c>
-      <c r="C84" s="2" t="inlineStr">
-        <is>
-          <t>11/07/2025</t>
-        </is>
-      </c>
-      <c r="D84" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="E84" s="2" t="n">
-        <v>48.54</v>
-      </c>
-      <c r="F84" s="2" t="inlineStr">
-        <is>
-          <t>7/49</t>
-        </is>
-      </c>
-      <c r="G84" s="2" t="n">
-        <v>240.19</v>
-      </c>
-      <c r="H84" s="2" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B85" s="3" t="inlineStr">
-        <is>
-          <t>11/07/2025</t>
-        </is>
-      </c>
-      <c r="C85" s="3" t="inlineStr">
-        <is>
-          <t>15/07/2025</t>
-        </is>
-      </c>
-      <c r="D85" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E85" s="3" t="n">
-        <v>-6.54</v>
-      </c>
-      <c r="F85" s="3" t="inlineStr">
-        <is>
-          <t>7/48</t>
-        </is>
-      </c>
-      <c r="G85" s="3" t="n">
-        <v>233.65</v>
-      </c>
-      <c r="H85" s="3" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B86" s="2" t="inlineStr">
-        <is>
-          <t>15/07/2025</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="inlineStr">
-        <is>
-          <t>22/07/2025</t>
-        </is>
-      </c>
-      <c r="D86" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E86" s="2" t="n">
-        <v>7.69</v>
-      </c>
-      <c r="F86" s="2" t="inlineStr">
-        <is>
-          <t>40/49</t>
-        </is>
-      </c>
-      <c r="G86" s="2" t="n">
-        <v>241.34</v>
-      </c>
-      <c r="H86" s="2" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B87" s="3" t="inlineStr">
-        <is>
-          <t>22/07/2025</t>
-        </is>
-      </c>
-      <c r="C87" s="3" t="inlineStr">
-        <is>
-          <t>07/08/2025</t>
-        </is>
-      </c>
-      <c r="D87" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E87" s="3" t="n">
-        <v>-16.23</v>
-      </c>
-      <c r="F87" s="3" t="inlineStr">
-        <is>
-          <t>24/48</t>
-        </is>
-      </c>
-      <c r="G87" s="3" t="n">
-        <v>225.11</v>
-      </c>
-      <c r="H87" s="3" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B88" s="2" t="inlineStr">
-        <is>
-          <t>07/08/2025</t>
-        </is>
-      </c>
-      <c r="C88" s="2" t="inlineStr">
-        <is>
-          <t>15/08/2025</t>
-        </is>
-      </c>
-      <c r="D88" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E88" s="2" t="n">
-        <v>21.71</v>
-      </c>
-      <c r="F88" s="2" t="inlineStr">
-        <is>
-          <t>16/49</t>
-        </is>
-      </c>
-      <c r="G88" s="2" t="n">
-        <v>246.82</v>
-      </c>
-      <c r="H88" s="2" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B89" s="3" t="inlineStr">
-        <is>
-          <t>15/08/2025</t>
-        </is>
-      </c>
-      <c r="C89" s="3" t="inlineStr">
-        <is>
-          <t>07/10/2025</t>
-        </is>
-      </c>
-      <c r="D89" s="3" t="n">
-        <v>36</v>
-      </c>
-      <c r="E89" s="3" t="n">
-        <v>-4.46</v>
-      </c>
-      <c r="F89" s="3" t="inlineStr">
-        <is>
-          <t>2/48</t>
-        </is>
-      </c>
-      <c r="G89" s="3" t="n">
-        <v>242.36</v>
-      </c>
-      <c r="H89" s="3" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B90" s="2" t="inlineStr">
-        <is>
-          <t>07/10/2025</t>
-        </is>
-      </c>
-      <c r="C90" s="2" t="inlineStr">
-        <is>
-          <t>17/10/2025</t>
-        </is>
-      </c>
-      <c r="D90" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="E90" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F90" s="2" t="inlineStr">
-        <is>
-          <t>45/49</t>
-        </is>
-      </c>
-      <c r="G90" s="2" t="n">
-        <v>246.36</v>
-      </c>
-      <c r="H90" s="2" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B91" s="3" t="inlineStr">
-        <is>
-          <t>17/10/2025</t>
-        </is>
-      </c>
-      <c r="C91" s="3" t="inlineStr">
-        <is>
-          <t>04/11/2025</t>
-        </is>
-      </c>
-      <c r="D91" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E91" s="3" t="n">
-        <v>-19.87</v>
-      </c>
-      <c r="F91" s="3" t="inlineStr">
-        <is>
-          <t>31/48</t>
-        </is>
-      </c>
-      <c r="G91" s="3" t="n">
-        <v>226.49</v>
-      </c>
-      <c r="H91" s="3" t="inlineStr"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B92" s="2" t="inlineStr">
-        <is>
-          <t>04/11/2025</t>
-        </is>
-      </c>
-      <c r="C92" s="2" t="inlineStr">
-        <is>
-          <t>14/11/2025</t>
-        </is>
-      </c>
-      <c r="D92" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="F92" s="2" t="inlineStr">
-        <is>
-          <t>20/49</t>
-        </is>
-      </c>
-      <c r="G92" s="2" t="n">
-        <v>244.09</v>
-      </c>
-      <c r="H92" s="2" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B93" s="3" t="inlineStr">
-        <is>
-          <t>14/11/2025</t>
-        </is>
-      </c>
-      <c r="C93" s="3" t="inlineStr">
-        <is>
-          <t>08/12/2025</t>
-        </is>
-      </c>
-      <c r="D93" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="E93" s="3" t="n">
-        <v>-16.33</v>
-      </c>
-      <c r="F93" s="3" t="inlineStr">
-        <is>
-          <t>25/48</t>
-        </is>
-      </c>
-      <c r="G93" s="3" t="n">
-        <v>227.76</v>
-      </c>
-      <c r="H93" s="3" t="inlineStr"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B94" s="2" t="inlineStr">
-        <is>
-          <t>08/12/2025</t>
-        </is>
-      </c>
-      <c r="C94" s="2" t="inlineStr">
-        <is>
-          <t>11/12/2025</t>
-        </is>
-      </c>
-      <c r="D94" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="F94" s="2" t="inlineStr">
-        <is>
-          <t>42/49</t>
-        </is>
-      </c>
-      <c r="G94" s="2" t="n">
-        <v>235.08</v>
-      </c>
-      <c r="H94" s="2" t="inlineStr"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B95" s="3" t="inlineStr">
-        <is>
-          <t>11/12/2025</t>
-        </is>
-      </c>
-      <c r="C95" s="3" t="inlineStr">
-        <is>
-          <t>16/12/2025</t>
-        </is>
-      </c>
-      <c r="D95" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E95" s="3" t="n">
-        <v>-11.36</v>
-      </c>
-      <c r="F95" s="3" t="inlineStr">
-        <is>
-          <t>17/48</t>
-        </is>
-      </c>
-      <c r="G95" s="3" t="n">
-        <v>223.72</v>
-      </c>
-      <c r="H95" s="3" t="inlineStr"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B96" s="2" t="inlineStr">
-        <is>
-          <t>16/12/2025</t>
-        </is>
-      </c>
-      <c r="C96" s="2" t="inlineStr">
-        <is>
-          <t>22/12/2025</t>
-        </is>
-      </c>
-      <c r="D96" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E96" s="2" t="n">
-        <v>4.27</v>
-      </c>
-      <c r="F96" s="2" t="inlineStr">
-        <is>
-          <t>44/49</t>
-        </is>
-      </c>
-      <c r="G96" s="2" t="n">
-        <v>227.99</v>
-      </c>
-      <c r="H96" s="2" t="inlineStr"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B97" s="3" t="inlineStr">
-        <is>
-          <t>22/12/2025</t>
-        </is>
-      </c>
-      <c r="C97" s="3" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
-      <c r="D97" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E97" s="3" t="n">
-        <v>-9.84</v>
-      </c>
-      <c r="F97" s="3" t="inlineStr">
-        <is>
-          <t>13/48</t>
-        </is>
-      </c>
-      <c r="G97" s="3" t="n">
-        <v>218.15</v>
-      </c>
-      <c r="H97" s="3" t="inlineStr"/>
-    </row>
-    <row r="98">
-      <c r="A98" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B98" s="2" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
-      <c r="C98" s="2" t="inlineStr">
-        <is>
-          <t>17/02/2026</t>
-        </is>
-      </c>
-      <c r="D98" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="E98" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="F98" s="2" t="inlineStr">
-        <is>
-          <t>9/49</t>
-        </is>
-      </c>
-      <c r="G98" s="2" t="n">
-        <v>258.15</v>
-      </c>
-      <c r="H98" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Improve backtest logic; refine CSV output formatting
Enhanced the insider conviction strategy backtest script and updated the accompanying CSV file for better clarity and data representation.

- Added price history tracking for rise start detection in backtest logic.
- Implemented event tracking for improved CSV/Excel output.
- Updated grov_rise_events.xlsx with refined data formatting.

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/grov_rise_events.xlsx
+++ b/output CSVs/grov_rise_events.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GROV Rise Events" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GROV Rise-Fall Events" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <col width="8" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
     <col width="8" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
     <col width="30" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -505,29 +505,29 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>26/08/2021</t>
+          <t>08/06/2021</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>06/06/2022</t>
+          <t>10/06/2021</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>196</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>3.21</v>
+        <v>1.23</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>38/39</t>
+          <t>57/58</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>3.21</v>
-      </c>
-      <c r="H2" s="2" t="inlineStr"/>
+        <v>1.23</v>
+      </c>
+      <c r="H2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -537,33 +537,29 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>06/06/2022</t>
+          <t>10/06/2021</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>20/07/2022</t>
+          <t>29/06/2021</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>-55.02</v>
+        <v>-1.31</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>36/38</t>
+          <t>54/58</t>
         </is>
       </c>
       <c r="G3" s="3" t="n">
-        <v>-51.81</v>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>16/06/2022</t>
-        </is>
-      </c>
+        <v>-0.09</v>
+      </c>
+      <c r="H3" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -573,29 +569,29 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>20/07/2022</t>
+          <t>29/06/2021</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>25/07/2022</t>
+          <t>05/08/2021</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2.9</v>
+        <v>0.41</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>39/39</t>
+          <t>58/58</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>-48.91</v>
-      </c>
-      <c r="H4" s="2" t="inlineStr"/>
+        <v>0.32</v>
+      </c>
+      <c r="H4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -605,29 +601,29 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>25/07/2022</t>
+          <t>05/08/2021</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>08/08/2022</t>
+          <t>07/09/2021</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>-10.41</v>
+        <v>-1.63</v>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>7/38</t>
+          <t>53/58</t>
         </is>
       </c>
       <c r="G5" s="3" t="n">
-        <v>-59.32</v>
-      </c>
-      <c r="H5" s="3" t="inlineStr"/>
+        <v>-1.31</v>
+      </c>
+      <c r="H5" s="3" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -637,29 +633,29 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>08/08/2022</t>
+          <t>07/09/2021</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>18/08/2022</t>
+          <t>04/11/2021</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>69.01000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>3/39</t>
+          <t>54/58</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>9.69</v>
-      </c>
-      <c r="H6" s="2" t="inlineStr"/>
+        <v>0.55</v>
+      </c>
+      <c r="H6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -669,33 +665,29 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>18/08/2022</t>
+          <t>04/11/2021</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>30/08/2022</t>
+          <t>06/12/2021</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>-32.66</v>
+        <v>-0.91</v>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>30/38</t>
+          <t>56/58</t>
         </is>
       </c>
       <c r="G7" s="3" t="n">
-        <v>-22.98</v>
-      </c>
-      <c r="H7" s="3" t="inlineStr">
-        <is>
-          <t>30/08/2022</t>
-        </is>
-      </c>
+        <v>-0.36</v>
+      </c>
+      <c r="H7" s="3" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -705,33 +697,29 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>30/08/2022</t>
+          <t>06/12/2021</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>16/09/2022</t>
+          <t>05/01/2022</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>47.87</v>
+        <v>1.53</v>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>7/39</t>
+          <t>55/58</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
-        <v>24.89</v>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>30/08/2022</t>
-        </is>
-      </c>
+        <v>1.17</v>
+      </c>
+      <c r="H8" s="2" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -741,29 +729,29 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>16/09/2022</t>
+          <t>05/01/2022</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>12/10/2022</t>
+          <t>19/01/2022</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>-79.42</v>
+        <v>-1.11</v>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>37/38</t>
+          <t>55/58</t>
         </is>
       </c>
       <c r="G9" s="3" t="n">
-        <v>-54.53</v>
-      </c>
-      <c r="H9" s="3" t="inlineStr"/>
+        <v>0.06</v>
+      </c>
+      <c r="H9" s="3" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
@@ -773,29 +761,29 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>12/10/2022</t>
+          <t>19/01/2022</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>19/10/2022</t>
+          <t>06/06/2022</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>11.89</v>
+        <v>1.32</v>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>28/39</t>
+          <t>56/58</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>-42.64</v>
-      </c>
-      <c r="H10" s="2" t="inlineStr"/>
+        <v>1.39</v>
+      </c>
+      <c r="H10" s="2" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -805,29 +793,29 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>19/10/2022</t>
+          <t>06/06/2022</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>03/11/2022</t>
+          <t>20/07/2022</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>-33.13</v>
+        <v>-59.84</v>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>31/38</t>
+          <t>3/58</t>
         </is>
       </c>
       <c r="G11" s="3" t="n">
-        <v>-75.77</v>
-      </c>
-      <c r="H11" s="3" t="inlineStr"/>
+        <v>-58.45</v>
+      </c>
+      <c r="H11" s="3" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
@@ -837,29 +825,29 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>03/11/2022</t>
+          <t>20/07/2022</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>09/11/2022</t>
+          <t>01/08/2022</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>17.76</v>
+        <v>4.91</v>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>20/39</t>
+          <t>47/58</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
-        <v>-58.01</v>
-      </c>
-      <c r="H12" s="2" t="inlineStr"/>
+        <v>-53.54</v>
+      </c>
+      <c r="H12" s="2" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
@@ -869,33 +857,29 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>09/11/2022</t>
+          <t>01/08/2022</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>20/12/2022</t>
+          <t>08/08/2022</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>-83.73</v>
+        <v>-12.13</v>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>38/38</t>
+          <t>31/58</t>
         </is>
       </c>
       <c r="G13" s="3" t="n">
-        <v>-141.74</v>
-      </c>
-      <c r="H13" s="3" t="inlineStr">
-        <is>
-          <t>05/12/2022, 22/11/2022</t>
-        </is>
-      </c>
+        <v>-65.67</v>
+      </c>
+      <c r="H13" s="3" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
@@ -905,29 +889,29 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>20/12/2022</t>
+          <t>08/08/2022</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>17/01/2023</t>
+          <t>18/08/2022</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>197.56</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>1/39</t>
+          <t>3/58</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
-        <v>55.82</v>
-      </c>
-      <c r="H14" s="2" t="inlineStr"/>
+        <v>3.34</v>
+      </c>
+      <c r="H14" s="2" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -937,29 +921,33 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>17/01/2023</t>
+          <t>18/08/2022</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>30/01/2023</t>
+          <t>01/09/2022</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>-29.51</v>
+        <v>-32.66</v>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>27/38</t>
+          <t>7/58</t>
         </is>
       </c>
       <c r="G15" s="3" t="n">
-        <v>26.32</v>
-      </c>
-      <c r="H15" s="3" t="inlineStr"/>
+        <v>-29.33</v>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>30/08/2022</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
@@ -969,29 +957,29 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>30/01/2023</t>
+          <t>01/09/2022</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>08/02/2023</t>
+          <t>16/09/2022</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>17.21</v>
+        <v>44.19</v>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>22/39</t>
+          <t>6/58</t>
         </is>
       </c>
       <c r="G16" s="2" t="n">
-        <v>43.53</v>
-      </c>
-      <c r="H16" s="2" t="inlineStr"/>
+        <v>14.86</v>
+      </c>
+      <c r="H16" s="2" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
@@ -1001,29 +989,29 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>08/02/2023</t>
+          <t>16/09/2022</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>22/02/2023</t>
+          <t>03/10/2022</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>-20.44</v>
+        <v>-68.06</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>22/38</t>
+          <t>2/58</t>
         </is>
       </c>
       <c r="G17" s="3" t="n">
-        <v>23.09</v>
-      </c>
-      <c r="H17" s="3" t="inlineStr"/>
+        <v>-53.2</v>
+      </c>
+      <c r="H17" s="3" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
@@ -1033,29 +1021,29 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>22/02/2023</t>
+          <t>03/10/2022</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>07/03/2023</t>
+          <t>05/10/2022</t>
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>39.65</v>
+        <v>4.95</v>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>9/39</t>
+          <t>46/58</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>62.74</v>
-      </c>
-      <c r="H18" s="2" t="inlineStr"/>
+        <v>-48.24</v>
+      </c>
+      <c r="H18" s="2" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
@@ -1065,33 +1053,29 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>07/03/2023</t>
+          <t>05/10/2022</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>20/03/2023</t>
+          <t>03/11/2022</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>-41.07</v>
+        <v>-54.08</v>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>34/38</t>
+          <t>4/58</t>
         </is>
       </c>
       <c r="G19" s="3" t="n">
-        <v>21.67</v>
-      </c>
-      <c r="H19" s="3" t="inlineStr">
-        <is>
-          <t>17/03/2023, 20/03/2023</t>
-        </is>
-      </c>
+        <v>-102.32</v>
+      </c>
+      <c r="H19" s="3" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
@@ -1101,33 +1085,29 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>20/03/2023</t>
+          <t>03/11/2022</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>04/04/2023</t>
+          <t>09/11/2022</t>
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>52.42</v>
+        <v>17.76</v>
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>5/39</t>
+          <t>21/58</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
-        <v>74.09</v>
-      </c>
-      <c r="H20" s="2" t="inlineStr">
-        <is>
-          <t>20/03/2023</t>
-        </is>
-      </c>
+        <v>-84.56</v>
+      </c>
+      <c r="H20" s="2" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
@@ -1137,29 +1117,33 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>04/04/2023</t>
+          <t>09/11/2022</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>11/04/2023</t>
+          <t>20/12/2022</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>-11.73</v>
+        <v>-83.73</v>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>8/38</t>
+          <t>1/58</t>
         </is>
       </c>
       <c r="G21" s="3" t="n">
-        <v>62.36</v>
-      </c>
-      <c r="H21" s="3" t="inlineStr"/>
+        <v>-168.29</v>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>22/11/2022, 05/12/2022</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
@@ -1169,29 +1153,29 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>11/04/2023</t>
+          <t>20/12/2022</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>28/04/2023</t>
+          <t>17/01/2023</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>10.36</v>
+        <v>197.56</v>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>29/39</t>
+          <t>1/58</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
-        <v>72.72</v>
-      </c>
-      <c r="H22" s="2" t="inlineStr"/>
+        <v>29.27</v>
+      </c>
+      <c r="H22" s="2" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
@@ -1201,29 +1185,29 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>28/04/2023</t>
+          <t>17/01/2023</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>16/05/2023</t>
+          <t>30/01/2023</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>-8.57</v>
+        <v>-29.51</v>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>5/38</t>
+          <t>9/58</t>
         </is>
       </c>
       <c r="G23" s="3" t="n">
-        <v>64.15000000000001</v>
-      </c>
-      <c r="H23" s="3" t="inlineStr"/>
+        <v>-0.24</v>
+      </c>
+      <c r="H23" s="3" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
@@ -1233,33 +1217,29 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>16/05/2023</t>
+          <t>30/01/2023</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>25/05/2023</t>
+          <t>06/02/2023</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>20.54</v>
+        <v>21.86</v>
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>17/39</t>
+          <t>15/58</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
-        <v>84.69</v>
-      </c>
-      <c r="H24" s="2" t="inlineStr">
-        <is>
-          <t>17/05/2023, 22/05/2023, 23/05/2023, 24/05/2023</t>
-        </is>
-      </c>
+        <v>21.62</v>
+      </c>
+      <c r="H24" s="2" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
@@ -1269,33 +1249,29 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>25/05/2023</t>
+          <t>06/02/2023</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>09/06/2023</t>
+          <t>01/03/2023</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>-33.7</v>
+        <v>-23.47</v>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>32/38</t>
+          <t>16/58</t>
         </is>
       </c>
       <c r="G25" s="3" t="n">
-        <v>50.98</v>
-      </c>
-      <c r="H25" s="3" t="inlineStr">
-        <is>
-          <t>01/06/2023, 09/06/2023, 26/05/2023, 30/05/2023</t>
-        </is>
-      </c>
+        <v>-1.85</v>
+      </c>
+      <c r="H25" s="3" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
@@ -1305,33 +1281,29 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>09/06/2023</t>
+          <t>01/03/2023</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>16/06/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="D26" s="2" t="n">
         <v>6</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>13.41</v>
+        <v>29.93</v>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>27/39</t>
+          <t>12/58</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>64.39</v>
-      </c>
-      <c r="H26" s="2" t="inlineStr">
-        <is>
-          <t>09/06/2023</t>
-        </is>
-      </c>
+        <v>28.08</v>
+      </c>
+      <c r="H26" s="2" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
@@ -1341,29 +1313,33 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>16/06/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>20/03/2023</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>-19.21</v>
+        <v>-41.07</v>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>18/38</t>
+          <t>6/58</t>
         </is>
       </c>
       <c r="G27" s="3" t="n">
-        <v>45.18</v>
-      </c>
-      <c r="H27" s="3" t="inlineStr"/>
+        <v>-12.99</v>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>17/03/2023</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
@@ -1373,29 +1349,29 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>20/03/2023</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>04/04/2023</t>
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>33.54</v>
+        <v>52.42</v>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>12/39</t>
+          <t>4/58</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>78.72</v>
-      </c>
-      <c r="H28" s="2" t="inlineStr"/>
+        <v>39.43</v>
+      </c>
+      <c r="H28" s="2" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
@@ -1405,29 +1381,29 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>04/04/2023</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>31/07/2023</t>
+          <t>13/04/2023</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>-15.53</v>
+        <v>-11.73</v>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>14/38</t>
+          <t>33/58</t>
         </is>
       </c>
       <c r="G29" s="3" t="n">
-        <v>63.2</v>
-      </c>
-      <c r="H29" s="3" t="inlineStr"/>
+        <v>27.7</v>
+      </c>
+      <c r="H29" s="3" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
@@ -1437,29 +1413,29 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>31/07/2023</t>
+          <t>13/04/2023</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>29/08/2023</t>
+          <t>18/04/2023</t>
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>94.05</v>
+        <v>11.56</v>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>2/39</t>
+          <t>30/58</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>157.25</v>
-      </c>
-      <c r="H30" s="2" t="inlineStr"/>
+        <v>39.26</v>
+      </c>
+      <c r="H30" s="2" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
@@ -1469,29 +1445,29 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>29/08/2023</t>
+          <t>18/04/2023</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>21/09/2023</t>
+          <t>26/04/2023</t>
         </is>
       </c>
       <c r="D31" s="3" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>-26.74</v>
+        <v>-10.36</v>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>25/38</t>
+          <t>37/58</t>
         </is>
       </c>
       <c r="G31" s="3" t="n">
-        <v>130.5</v>
-      </c>
-      <c r="H31" s="3" t="inlineStr"/>
+        <v>28.9</v>
+      </c>
+      <c r="H31" s="3" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
@@ -1501,29 +1477,29 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>21/09/2023</t>
+          <t>26/04/2023</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>26/09/2023</t>
+          <t>28/04/2023</t>
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>6.08</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>36/39</t>
+          <t>36/58</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
-        <v>136.58</v>
-      </c>
-      <c r="H32" s="2" t="inlineStr"/>
+        <v>37.79</v>
+      </c>
+      <c r="H32" s="2" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
@@ -1533,29 +1509,33 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>26/09/2023</t>
+          <t>28/04/2023</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>13/10/2023</t>
+          <t>09/06/2023</t>
         </is>
       </c>
       <c r="D33" s="3" t="n">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>-41.94</v>
+        <v>-26.94</v>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>35/38</t>
+          <t>11/58</t>
         </is>
       </c>
       <c r="G33" s="3" t="n">
-        <v>94.65000000000001</v>
-      </c>
-      <c r="H33" s="3" t="inlineStr"/>
+        <v>10.85</v>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>17/05/2023, 22/05/2023, 23/05/2023, 24/05/2023, 26/05/2023, 30/05/2023, 01/06/2023</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
@@ -1565,29 +1545,29 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>13/10/2023</t>
+          <t>09/06/2023</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>19/10/2023</t>
+          <t>13/06/2023</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>16.67</v>
+        <v>18.44</v>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>23/39</t>
+          <t>18/58</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>111.32</v>
-      </c>
-      <c r="H34" s="2" t="inlineStr"/>
+        <v>29.29</v>
+      </c>
+      <c r="H34" s="2" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
@@ -1597,29 +1577,29 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>19/10/2023</t>
+          <t>13/06/2023</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>01/11/2023</t>
+          <t>27/06/2023</t>
         </is>
       </c>
       <c r="D35" s="3" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E35" s="3" t="n">
-        <v>-19.58</v>
+        <v>-22.64</v>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>19/38</t>
+          <t>17/58</t>
         </is>
       </c>
       <c r="G35" s="3" t="n">
-        <v>91.73999999999999</v>
-      </c>
-      <c r="H35" s="3" t="inlineStr"/>
+        <v>6.64</v>
+      </c>
+      <c r="H35" s="3" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
@@ -1629,29 +1609,29 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>01/11/2023</t>
+          <t>27/06/2023</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>22/11/2023</t>
+          <t>12/07/2023</t>
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>53.95</v>
+        <v>33.54</v>
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>4/39</t>
+          <t>9/58</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>145.69</v>
-      </c>
-      <c r="H36" s="2" t="inlineStr"/>
+        <v>40.18</v>
+      </c>
+      <c r="H36" s="2" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
@@ -1661,33 +1641,29 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>22/11/2023</t>
+          <t>12/07/2023</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>03/08/2023</t>
         </is>
       </c>
       <c r="D37" s="3" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>-22.22</v>
+        <v>-15.53</v>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>23/38</t>
+          <t>26/58</t>
         </is>
       </c>
       <c r="G37" s="3" t="n">
-        <v>123.47</v>
-      </c>
-      <c r="H37" s="3" t="inlineStr">
-        <is>
-          <t>14/12/2023</t>
-        </is>
-      </c>
+        <v>24.66</v>
+      </c>
+      <c r="H37" s="3" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
@@ -1697,29 +1673,29 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>03/08/2023</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>18/08/2023</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>16.48</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>24/39</t>
+          <t>2/58</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>139.95</v>
-      </c>
-      <c r="H38" s="2" t="inlineStr"/>
+        <v>102.67</v>
+      </c>
+      <c r="H38" s="2" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
@@ -1729,29 +1705,29 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>18/08/2023</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>26/01/2024</t>
+          <t>24/08/2023</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>-19.81</v>
+        <v>-8.529999999999999</v>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>20/38</t>
+          <t>43/58</t>
         </is>
       </c>
       <c r="G39" s="3" t="n">
-        <v>120.14</v>
-      </c>
-      <c r="H39" s="3" t="inlineStr"/>
+        <v>94.14</v>
+      </c>
+      <c r="H39" s="3" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
@@ -1761,29 +1737,29 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>26/01/2024</t>
+          <t>24/08/2023</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>31/01/2024</t>
+          <t>29/08/2023</t>
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>7.65</v>
+        <v>15.43</v>
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>33/39</t>
+          <t>24/58</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>127.79</v>
-      </c>
-      <c r="H40" s="2" t="inlineStr"/>
+        <v>109.57</v>
+      </c>
+      <c r="H40" s="2" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
@@ -1793,29 +1769,29 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>31/01/2024</t>
+          <t>29/08/2023</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>13/09/2023</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>-9.84</v>
+        <v>-23.96</v>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>6/38</t>
+          <t>15/58</t>
         </is>
       </c>
       <c r="G41" s="3" t="n">
-        <v>117.95</v>
-      </c>
-      <c r="H41" s="3" t="inlineStr"/>
+        <v>85.62</v>
+      </c>
+      <c r="H41" s="3" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
@@ -1825,29 +1801,29 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>13/09/2023</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>05/03/2024</t>
+          <t>15/09/2023</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>39.39</v>
+        <v>17.22</v>
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>10/39</t>
+          <t>22/58</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>157.34</v>
-      </c>
-      <c r="H42" s="2" t="inlineStr"/>
+        <v>102.83</v>
+      </c>
+      <c r="H42" s="2" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
@@ -1857,33 +1833,29 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>05/03/2024</t>
+          <t>15/09/2023</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>03/04/2024</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>-32.61</v>
+        <v>-49.38</v>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>29/38</t>
+          <t>5/58</t>
         </is>
       </c>
       <c r="G43" s="3" t="n">
-        <v>124.73</v>
-      </c>
-      <c r="H43" s="3" t="inlineStr">
-        <is>
-          <t>08/03/2024, 11/03/2024</t>
-        </is>
-      </c>
+        <v>53.46</v>
+      </c>
+      <c r="H43" s="3" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
@@ -1893,29 +1865,29 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>03/04/2024</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>08/04/2024</t>
+          <t>19/10/2023</t>
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>9.68</v>
+        <v>16.67</v>
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>31/39</t>
+          <t>23/58</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>134.41</v>
-      </c>
-      <c r="H44" s="2" t="inlineStr"/>
+        <v>70.12</v>
+      </c>
+      <c r="H44" s="2" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
@@ -1925,29 +1897,29 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>08/04/2024</t>
+          <t>19/10/2023</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>15/04/2024</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>-15.29</v>
+        <v>-19.58</v>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>13/38</t>
+          <t>21/58</t>
         </is>
       </c>
       <c r="G45" s="3" t="n">
-        <v>119.12</v>
-      </c>
-      <c r="H45" s="3" t="inlineStr"/>
+        <v>50.55</v>
+      </c>
+      <c r="H45" s="3" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
@@ -1957,29 +1929,29 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>15/04/2024</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>09/05/2024</t>
+          <t>22/11/2023</t>
         </is>
       </c>
       <c r="D46" s="2" t="n">
         <v>19</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>18.75</v>
+        <v>50</v>
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>19/39</t>
+          <t>5/58</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
-        <v>137.87</v>
-      </c>
-      <c r="H46" s="2" t="inlineStr"/>
+        <v>100.55</v>
+      </c>
+      <c r="H46" s="2" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
@@ -1989,29 +1961,29 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>09/05/2024</t>
+          <t>22/11/2023</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>23/05/2024</t>
+          <t>12/12/2023</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>-14.04</v>
+        <v>-27.35</v>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>11/38</t>
+          <t>10/58</t>
         </is>
       </c>
       <c r="G47" s="3" t="n">
-        <v>123.83</v>
-      </c>
-      <c r="H47" s="3" t="inlineStr"/>
+        <v>73.2</v>
+      </c>
+      <c r="H47" s="3" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
@@ -2021,31 +1993,31 @@
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>23/05/2024</t>
+          <t>12/12/2023</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>05/06/2024</t>
+          <t>14/12/2023</t>
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>10.2</v>
+        <v>12.35</v>
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>30/39</t>
+          <t>28/58</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>134.03</v>
+        <v>85.55</v>
       </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
-          <t>29/05/2024</t>
+          <t>14/12/2023</t>
         </is>
       </c>
     </row>
@@ -2057,29 +2029,29 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>05/06/2024</t>
+          <t>14/12/2023</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>10/06/2024</t>
+          <t>20/12/2023</t>
         </is>
       </c>
       <c r="D49" s="3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>-5.56</v>
+        <v>-4.71</v>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>3/38</t>
+          <t>50/58</t>
         </is>
       </c>
       <c r="G49" s="3" t="n">
-        <v>128.48</v>
-      </c>
-      <c r="H49" s="3" t="inlineStr"/>
+        <v>80.84</v>
+      </c>
+      <c r="H49" s="3" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
@@ -2089,29 +2061,29 @@
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>10/06/2024</t>
+          <t>20/12/2023</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>03/07/2024</t>
+          <t>22/12/2023</t>
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>20.26</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>18/39</t>
+          <t>33/58</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>148.74</v>
-      </c>
-      <c r="H50" s="2" t="inlineStr"/>
+        <v>90.73</v>
+      </c>
+      <c r="H50" s="2" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
@@ -2121,29 +2093,29 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>03/07/2024</t>
+          <t>22/12/2023</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>28/08/2024</t>
+          <t>29/12/2023</t>
         </is>
       </c>
       <c r="D51" s="3" t="n">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>-30.98</v>
+        <v>-11.5</v>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>28/38</t>
+          <t>35/58</t>
         </is>
       </c>
       <c r="G51" s="3" t="n">
-        <v>117.76</v>
-      </c>
-      <c r="H51" s="3" t="inlineStr"/>
+        <v>79.23</v>
+      </c>
+      <c r="H51" s="3" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
@@ -2153,29 +2125,29 @@
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>28/08/2024</t>
+          <t>29/12/2023</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>14.17</v>
+        <v>19.77</v>
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>26/39</t>
+          <t>16/58</t>
         </is>
       </c>
       <c r="G52" s="2" t="n">
-        <v>131.93</v>
-      </c>
-      <c r="H52" s="2" t="inlineStr"/>
+        <v>99</v>
+      </c>
+      <c r="H52" s="2" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
@@ -2185,29 +2157,29 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>26/01/2024</t>
         </is>
       </c>
       <c r="D53" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>-12.41</v>
+        <v>-19.81</v>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>9/38</t>
+          <t>19/58</t>
         </is>
       </c>
       <c r="G53" s="3" t="n">
-        <v>119.52</v>
-      </c>
-      <c r="H53" s="3" t="inlineStr"/>
+        <v>79.19</v>
+      </c>
+      <c r="H53" s="3" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
@@ -2217,29 +2189,29 @@
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>26/01/2024</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>31/01/2024</t>
         </is>
       </c>
       <c r="D54" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>14.96</v>
+        <v>7.65</v>
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>25/39</t>
+          <t>39/58</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
-        <v>134.48</v>
-      </c>
-      <c r="H54" s="2" t="inlineStr"/>
+        <v>86.84</v>
+      </c>
+      <c r="H54" s="2" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
@@ -2249,29 +2221,29 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>31/01/2024</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>30/10/2024</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="D55" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>-13.7</v>
+        <v>-9.84</v>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>10/38</t>
+          <t>38/58</t>
         </is>
       </c>
       <c r="G55" s="3" t="n">
-        <v>120.78</v>
-      </c>
-      <c r="H55" s="3" t="inlineStr"/>
+        <v>77</v>
+      </c>
+      <c r="H55" s="3" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
@@ -2281,29 +2253,29 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>30/10/2024</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>08/02/2024</t>
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>20.63</v>
+        <v>10.3</v>
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>16/39</t>
+          <t>32/58</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
-        <v>141.41</v>
-      </c>
-      <c r="H56" s="2" t="inlineStr"/>
+        <v>87.3</v>
+      </c>
+      <c r="H56" s="2" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
@@ -2313,29 +2285,29 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>08/02/2024</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>15/11/2024</t>
+          <t>22/02/2024</t>
         </is>
       </c>
       <c r="D57" s="3" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>-15.13</v>
+        <v>-8.789999999999999</v>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>12/38</t>
+          <t>41/58</t>
         </is>
       </c>
       <c r="G57" s="3" t="n">
-        <v>126.28</v>
-      </c>
-      <c r="H57" s="3" t="inlineStr"/>
+        <v>78.51000000000001</v>
+      </c>
+      <c r="H57" s="3" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
@@ -2345,33 +2317,29 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>15/11/2024</t>
+          <t>22/02/2024</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>08/01/2025</t>
+          <t>05/03/2024</t>
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>36.43</v>
+        <v>36.9</v>
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>11/39</t>
+          <t>8/58</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
-        <v>162.71</v>
-      </c>
-      <c r="H58" s="2" t="inlineStr">
-        <is>
-          <t>18/11/2024</t>
-        </is>
-      </c>
+        <v>115.42</v>
+      </c>
+      <c r="H58" s="2" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
@@ -2381,29 +2349,29 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>08/01/2025</t>
+          <t>05/03/2024</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>15/01/2025</t>
+          <t>03/04/2024</t>
         </is>
       </c>
       <c r="D59" s="3" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>-26.14</v>
+        <v>-32.61</v>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>24/38</t>
+          <t>8/58</t>
         </is>
       </c>
       <c r="G59" s="3" t="n">
-        <v>136.57</v>
-      </c>
-      <c r="H59" s="3" t="inlineStr"/>
+        <v>82.81</v>
+      </c>
+      <c r="H59" s="3" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
@@ -2413,29 +2381,29 @@
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>15/01/2025</t>
+          <t>03/04/2024</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>05/02/2025</t>
+          <t>08/04/2024</t>
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>31.54</v>
+        <v>9.68</v>
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>14/39</t>
+          <t>34/58</t>
         </is>
       </c>
       <c r="G60" s="2" t="n">
-        <v>168.11</v>
-      </c>
-      <c r="H60" s="2" t="inlineStr"/>
+        <v>92.48999999999999</v>
+      </c>
+      <c r="H60" s="2" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
@@ -2445,29 +2413,29 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>05/02/2025</t>
+          <t>08/04/2024</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>17/04/2024</t>
         </is>
       </c>
       <c r="D61" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>-8.19</v>
+        <v>-15.29</v>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>4/38</t>
+          <t>27/58</t>
         </is>
       </c>
       <c r="G61" s="3" t="n">
-        <v>159.92</v>
-      </c>
-      <c r="H61" s="3" t="inlineStr"/>
+        <v>77.19</v>
+      </c>
+      <c r="H61" s="3" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
@@ -2477,29 +2445,29 @@
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>17/04/2024</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>13/03/2025</t>
+          <t>22/04/2024</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>6.37</v>
+        <v>7.89</v>
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>35/39</t>
+          <t>38/58</t>
         </is>
       </c>
       <c r="G62" s="2" t="n">
-        <v>166.29</v>
-      </c>
-      <c r="H62" s="2" t="inlineStr"/>
+        <v>85.09</v>
+      </c>
+      <c r="H62" s="2" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
@@ -2509,29 +2477,29 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>13/03/2025</t>
+          <t>22/04/2024</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>11/04/2025</t>
+          <t>30/04/2024</t>
         </is>
       </c>
       <c r="D63" s="3" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>-37.13</v>
+        <v>-8.539999999999999</v>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>33/38</t>
+          <t>42/58</t>
         </is>
       </c>
       <c r="G63" s="3" t="n">
-        <v>129.17</v>
-      </c>
-      <c r="H63" s="3" t="inlineStr"/>
+        <v>76.55</v>
+      </c>
+      <c r="H63" s="3" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
@@ -2541,29 +2509,29 @@
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>11/04/2025</t>
+          <t>30/04/2024</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>09/05/2024</t>
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>8.57</v>
+        <v>14</v>
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>32/39</t>
+          <t>26/58</t>
         </is>
       </c>
       <c r="G64" s="2" t="n">
-        <v>137.74</v>
-      </c>
-      <c r="H64" s="2" t="inlineStr"/>
+        <v>90.55</v>
+      </c>
+      <c r="H64" s="2" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
@@ -2573,29 +2541,29 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>29/04/2025</t>
+          <t>09/05/2024</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>06/05/2025</t>
+          <t>16/05/2024</t>
         </is>
       </c>
       <c r="D65" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>-5.26</v>
+        <v>-12.87</v>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>2/38</t>
+          <t>29/58</t>
         </is>
       </c>
       <c r="G65" s="3" t="n">
-        <v>132.47</v>
-      </c>
-      <c r="H65" s="3" t="inlineStr"/>
+        <v>77.68000000000001</v>
+      </c>
+      <c r="H65" s="3" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
@@ -2605,31 +2573,31 @@
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>06/05/2025</t>
+          <t>16/05/2024</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>27/05/2025</t>
+          <t>14/06/2024</t>
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>32.41</v>
+        <v>18.12</v>
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>13/39</t>
+          <t>20/58</t>
         </is>
       </c>
       <c r="G66" s="2" t="n">
-        <v>164.88</v>
+        <v>95.81</v>
       </c>
       <c r="H66" s="2" t="inlineStr">
         <is>
-          <t>20/05/2025, 21/05/2025, 22/05/2025, 23/05/2025, 27/05/2025</t>
+          <t>29/05/2024</t>
         </is>
       </c>
     </row>
@@ -2641,33 +2609,29 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>27/05/2025</t>
+          <t>14/06/2024</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>25/06/2024</t>
         </is>
       </c>
       <c r="D67" s="3" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>-27.97</v>
+        <v>-9.09</v>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>26/38</t>
+          <t>40/58</t>
         </is>
       </c>
       <c r="G67" s="3" t="n">
-        <v>136.91</v>
-      </c>
-      <c r="H67" s="3" t="inlineStr">
-        <is>
-          <t>02/06/2025, 06/06/2025, 09/06/2025, 10/06/2025, 12/06/2025, 13/06/2025, 27/05/2025, 28/05/2025, 29/05/2025</t>
-        </is>
-      </c>
+        <v>86.70999999999999</v>
+      </c>
+      <c r="H67" s="3" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
@@ -2677,29 +2641,29 @@
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>25/06/2024</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>11/07/2025</t>
+          <t>03/07/2024</t>
         </is>
       </c>
       <c r="D68" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E68" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="E68" s="2" t="n">
-        <v>48.54</v>
-      </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>6/39</t>
+          <t>25/58</t>
         </is>
       </c>
       <c r="G68" s="2" t="n">
-        <v>185.45</v>
-      </c>
-      <c r="H68" s="2" t="inlineStr"/>
+        <v>101.71</v>
+      </c>
+      <c r="H68" s="2" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
@@ -2709,29 +2673,29 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>11/07/2025</t>
+          <t>03/07/2024</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>07/08/2025</t>
+          <t>05/08/2024</t>
         </is>
       </c>
       <c r="D69" s="3" t="n">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>-15.69</v>
+        <v>-26.63</v>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>15/38</t>
+          <t>12/58</t>
         </is>
       </c>
       <c r="G69" s="3" t="n">
-        <v>169.77</v>
-      </c>
-      <c r="H69" s="3" t="inlineStr"/>
+        <v>75.08</v>
+      </c>
+      <c r="H69" s="3" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
@@ -2741,29 +2705,29 @@
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>07/08/2025</t>
+          <t>05/08/2024</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>15/08/2025</t>
+          <t>08/08/2024</t>
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>21.71</v>
+        <v>5.93</v>
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>15/39</t>
+          <t>45/58</t>
         </is>
       </c>
       <c r="G70" s="2" t="n">
-        <v>191.48</v>
-      </c>
-      <c r="H70" s="2" t="inlineStr"/>
+        <v>81.01000000000001</v>
+      </c>
+      <c r="H70" s="2" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
@@ -2773,29 +2737,29 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>15/08/2025</t>
+          <t>08/08/2024</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>07/10/2025</t>
+          <t>14/08/2024</t>
         </is>
       </c>
       <c r="D71" s="3" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>-4.46</v>
+        <v>-11.19</v>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>1/38</t>
+          <t>36/58</t>
         </is>
       </c>
       <c r="G71" s="3" t="n">
-        <v>187.02</v>
-      </c>
-      <c r="H71" s="3" t="inlineStr"/>
+        <v>69.81999999999999</v>
+      </c>
+      <c r="H71" s="3" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
@@ -2805,29 +2769,29 @@
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>07/10/2025</t>
+          <t>14/08/2024</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>17/10/2025</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>4</v>
+        <v>7.09</v>
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>37/39</t>
+          <t>42/58</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
-        <v>191.02</v>
-      </c>
-      <c r="H72" s="2" t="inlineStr"/>
+        <v>76.91</v>
+      </c>
+      <c r="H72" s="2" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
@@ -2837,29 +2801,29 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>17/10/2025</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t>04/11/2025</t>
+          <t>30/08/2024</t>
         </is>
       </c>
       <c r="D73" s="3" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E73" s="3" t="n">
-        <v>-19.87</v>
+        <v>-6.62</v>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>21/38</t>
+          <t>45/58</t>
         </is>
       </c>
       <c r="G73" s="3" t="n">
-        <v>171.15</v>
-      </c>
-      <c r="H73" s="3" t="inlineStr"/>
+        <v>70.29000000000001</v>
+      </c>
+      <c r="H73" s="3" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="2" t="inlineStr">
@@ -2869,29 +2833,29 @@
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>04/11/2025</t>
+          <t>30/08/2024</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>14/11/2025</t>
+          <t>04/09/2024</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>17.6</v>
+        <v>3.88</v>
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>21/39</t>
+          <t>49/58</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
-        <v>188.75</v>
-      </c>
-      <c r="H74" s="2" t="inlineStr"/>
+        <v>74.17</v>
+      </c>
+      <c r="H74" s="2" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
@@ -2901,29 +2865,29 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>14/11/2025</t>
+          <t>04/09/2024</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>08/12/2025</t>
+          <t>11/09/2024</t>
         </is>
       </c>
       <c r="D75" s="3" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E75" s="3" t="n">
-        <v>-16.33</v>
+        <v>-0.75</v>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>16/38</t>
+          <t>58/58</t>
         </is>
       </c>
       <c r="G75" s="3" t="n">
-        <v>172.42</v>
-      </c>
-      <c r="H75" s="3" t="inlineStr"/>
+        <v>73.42</v>
+      </c>
+      <c r="H75" s="3" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="2" t="inlineStr">
@@ -2933,29 +2897,29 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>08/12/2025</t>
+          <t>11/09/2024</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>19/09/2024</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>7.32</v>
+        <v>9.02</v>
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>34/39</t>
+          <t>35/58</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
-        <v>179.74</v>
-      </c>
-      <c r="H76" s="2" t="inlineStr"/>
+        <v>82.44</v>
+      </c>
+      <c r="H76" s="2" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
@@ -2965,29 +2929,29 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>19/09/2024</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>31/12/2025</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="D77" s="3" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>-16.67</v>
+        <v>-11.72</v>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>17/38</t>
+          <t>34/58</t>
         </is>
       </c>
       <c r="G77" s="3" t="n">
-        <v>163.07</v>
-      </c>
-      <c r="H77" s="3" t="inlineStr"/>
+        <v>70.72</v>
+      </c>
+      <c r="H77" s="3" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="2" t="inlineStr">
@@ -2997,29 +2961,1285 @@
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="inlineStr">
+        <is>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="F78" s="2" t="inlineStr">
+        <is>
+          <t>52/58</t>
+        </is>
+      </c>
+      <c r="G78" s="2" t="n">
+        <v>73.84</v>
+      </c>
+      <c r="H78" s="2" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B79" s="3" t="inlineStr">
+        <is>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C79" s="3" t="inlineStr">
+        <is>
+          <t>01/11/2024</t>
+        </is>
+      </c>
+      <c r="D79" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E79" s="3" t="n">
+        <v>-4.55</v>
+      </c>
+      <c r="F79" s="3" t="inlineStr">
+        <is>
+          <t>51/58</t>
+        </is>
+      </c>
+      <c r="G79" s="3" t="n">
+        <v>69.3</v>
+      </c>
+      <c r="H79" s="3" t="n"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>01/11/2024</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>12/11/2024</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E80" s="2" t="n">
+        <v>18.75</v>
+      </c>
+      <c r="F80" s="2" t="inlineStr">
+        <is>
+          <t>17/58</t>
+        </is>
+      </c>
+      <c r="G80" s="2" t="n">
+        <v>88.05</v>
+      </c>
+      <c r="H80" s="2" t="n"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B81" s="3" t="inlineStr">
+        <is>
+          <t>12/11/2024</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="inlineStr">
+        <is>
+          <t>26/11/2024</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E81" s="3" t="n">
+        <v>-13.82</v>
+      </c>
+      <c r="F81" s="3" t="inlineStr">
+        <is>
+          <t>28/58</t>
+        </is>
+      </c>
+      <c r="G81" s="3" t="n">
+        <v>74.23</v>
+      </c>
+      <c r="H81" s="3" t="n"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>26/11/2024</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr">
+        <is>
+          <t>29/11/2024</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>18.32</v>
+      </c>
+      <c r="F82" s="2" t="inlineStr">
+        <is>
+          <t>19/58</t>
+        </is>
+      </c>
+      <c r="G82" s="2" t="n">
+        <v>92.55</v>
+      </c>
+      <c r="H82" s="2" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B83" s="3" t="inlineStr">
+        <is>
+          <t>29/11/2024</t>
+        </is>
+      </c>
+      <c r="C83" s="3" t="inlineStr">
+        <is>
+          <t>23/12/2024</t>
+        </is>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>-12.26</v>
+      </c>
+      <c r="F83" s="3" t="inlineStr">
+        <is>
+          <t>30/58</t>
+        </is>
+      </c>
+      <c r="G83" s="3" t="n">
+        <v>80.29000000000001</v>
+      </c>
+      <c r="H83" s="3" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>23/12/2024</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>08/01/2025</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>29.41</v>
+      </c>
+      <c r="F84" s="2" t="inlineStr">
+        <is>
+          <t>13/58</t>
+        </is>
+      </c>
+      <c r="G84" s="2" t="n">
+        <v>109.71</v>
+      </c>
+      <c r="H84" s="2" t="n"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B85" s="3" t="inlineStr">
+        <is>
+          <t>08/01/2025</t>
+        </is>
+      </c>
+      <c r="C85" s="3" t="inlineStr">
+        <is>
+          <t>30/01/2025</t>
+        </is>
+      </c>
+      <c r="D85" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>-24.43</v>
+      </c>
+      <c r="F85" s="3" t="inlineStr">
+        <is>
+          <t>14/58</t>
+        </is>
+      </c>
+      <c r="G85" s="3" t="n">
+        <v>85.27</v>
+      </c>
+      <c r="H85" s="3" t="n"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr">
+        <is>
+          <t>30/01/2025</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>05/02/2025</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>23.02</v>
+      </c>
+      <c r="F86" s="2" t="inlineStr">
+        <is>
+          <t>14/58</t>
+        </is>
+      </c>
+      <c r="G86" s="2" t="n">
+        <v>108.3</v>
+      </c>
+      <c r="H86" s="2" t="n"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B87" s="3" t="inlineStr">
+        <is>
+          <t>05/02/2025</t>
+        </is>
+      </c>
+      <c r="C87" s="3" t="inlineStr">
+        <is>
+          <t>26/02/2025</t>
+        </is>
+      </c>
+      <c r="D87" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="E87" s="3" t="n">
+        <v>-6.43</v>
+      </c>
+      <c r="F87" s="3" t="inlineStr">
+        <is>
+          <t>46/58</t>
+        </is>
+      </c>
+      <c r="G87" s="3" t="n">
+        <v>101.86</v>
+      </c>
+      <c r="H87" s="3" t="n"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
+        <is>
+          <t>26/02/2025</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>28/02/2025</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="F88" s="2" t="inlineStr">
+        <is>
+          <t>53/58</t>
+        </is>
+      </c>
+      <c r="G88" s="2" t="n">
+        <v>104.35</v>
+      </c>
+      <c r="H88" s="2" t="n"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B89" s="3" t="inlineStr">
+        <is>
+          <t>28/02/2025</t>
+        </is>
+      </c>
+      <c r="C89" s="3" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
+      <c r="D89" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="E89" s="3" t="n">
+        <v>-18.79</v>
+      </c>
+      <c r="F89" s="3" t="inlineStr">
+        <is>
+          <t>22/58</t>
+        </is>
+      </c>
+      <c r="G89" s="3" t="n">
+        <v>85.56</v>
+      </c>
+      <c r="H89" s="3" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="F90" s="2" t="inlineStr">
+        <is>
+          <t>50/58</t>
+        </is>
+      </c>
+      <c r="G90" s="2" t="n">
+        <v>89.29000000000001</v>
+      </c>
+      <c r="H90" s="2" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B91" s="3" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
+      <c r="C91" s="3" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="D91" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E91" s="3" t="n">
+        <v>-24.46</v>
+      </c>
+      <c r="F91" s="3" t="inlineStr">
+        <is>
+          <t>13/58</t>
+        </is>
+      </c>
+      <c r="G91" s="3" t="n">
+        <v>64.83</v>
+      </c>
+      <c r="H91" s="3" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
+        <is>
+          <t>15/04/2025</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="F92" s="2" t="inlineStr">
+        <is>
+          <t>44/58</t>
+        </is>
+      </c>
+      <c r="G92" s="2" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="H92" s="2" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>15/04/2025</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="inlineStr">
+        <is>
+          <t>22/04/2025</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E93" s="3" t="n">
+        <v>-6.25</v>
+      </c>
+      <c r="F93" s="3" t="inlineStr">
+        <is>
+          <t>47/58</t>
+        </is>
+      </c>
+      <c r="G93" s="3" t="n">
+        <v>65.25</v>
+      </c>
+      <c r="H93" s="3" t="n"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
+        <is>
+          <t>22/04/2025</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>8.57</v>
+      </c>
+      <c r="F94" s="2" t="inlineStr">
+        <is>
+          <t>37/58</t>
+        </is>
+      </c>
+      <c r="G94" s="2" t="n">
+        <v>73.81999999999999</v>
+      </c>
+      <c r="H94" s="2" t="n"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B95" s="3" t="inlineStr">
+        <is>
+          <t>29/04/2025</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E95" s="3" t="n">
+        <v>-5.26</v>
+      </c>
+      <c r="F95" s="3" t="inlineStr">
+        <is>
+          <t>48/58</t>
+        </is>
+      </c>
+      <c r="G95" s="3" t="n">
+        <v>68.56</v>
+      </c>
+      <c r="H95" s="3" t="n"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>12/05/2025</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>12.96</v>
+      </c>
+      <c r="F96" s="2" t="inlineStr">
+        <is>
+          <t>27/58</t>
+        </is>
+      </c>
+      <c r="G96" s="2" t="n">
+        <v>81.52</v>
+      </c>
+      <c r="H96" s="2" t="n"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>12/05/2025</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="D97" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E97" s="3" t="n">
+        <v>-9.84</v>
+      </c>
+      <c r="F97" s="3" t="inlineStr">
+        <is>
+          <t>39/58</t>
+        </is>
+      </c>
+      <c r="G97" s="3" t="n">
+        <v>71.68000000000001</v>
+      </c>
+      <c r="H97" s="3" t="n"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>27/05/2025</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="F98" s="2" t="inlineStr">
+        <is>
+          <t>11/58</t>
+        </is>
+      </c>
+      <c r="G98" s="2" t="n">
+        <v>101.68</v>
+      </c>
+      <c r="H98" s="2" t="inlineStr">
+        <is>
+          <t>23/05/2025, 27/05/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B99" s="3" t="inlineStr">
+        <is>
+          <t>27/05/2025</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="inlineStr">
+        <is>
+          <t>12/06/2025</t>
+        </is>
+      </c>
+      <c r="D99" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E99" s="3" t="n">
+        <v>-21.68</v>
+      </c>
+      <c r="F99" s="3" t="inlineStr">
+        <is>
+          <t>18/58</t>
+        </is>
+      </c>
+      <c r="G99" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="H99" s="3" t="inlineStr">
+        <is>
+          <t>02/06/2025, 06/06/2025, 09/06/2025, 10/06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>12/06/2025</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
+        <is>
+          <t>16/06/2025</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>4.46</v>
+      </c>
+      <c r="F100" s="2" t="inlineStr">
+        <is>
+          <t>48/58</t>
+        </is>
+      </c>
+      <c r="G100" s="2" t="n">
+        <v>84.47</v>
+      </c>
+      <c r="H100" s="2" t="n"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B101" s="3" t="inlineStr">
+        <is>
+          <t>16/06/2025</t>
+        </is>
+      </c>
+      <c r="C101" s="3" t="inlineStr">
+        <is>
+          <t>20/06/2025</t>
+        </is>
+      </c>
+      <c r="D101" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E101" s="3" t="n">
+        <v>-11.97</v>
+      </c>
+      <c r="F101" s="3" t="inlineStr">
+        <is>
+          <t>32/58</t>
+        </is>
+      </c>
+      <c r="G101" s="3" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="H101" s="3" t="n"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="inlineStr">
+        <is>
+          <t>20/06/2025</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>25/06/2025</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>11.65</v>
+      </c>
+      <c r="F102" s="2" t="inlineStr">
+        <is>
+          <t>29/58</t>
+        </is>
+      </c>
+      <c r="G102" s="2" t="n">
+        <v>84.15000000000001</v>
+      </c>
+      <c r="H102" s="2" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B103" s="3" t="inlineStr">
+        <is>
+          <t>25/06/2025</t>
+        </is>
+      </c>
+      <c r="C103" s="3" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+      <c r="D103" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E103" s="3" t="n">
+        <v>-0.87</v>
+      </c>
+      <c r="F103" s="3" t="inlineStr">
+        <is>
+          <t>57/58</t>
+        </is>
+      </c>
+      <c r="G103" s="3" t="n">
+        <v>83.28</v>
+      </c>
+      <c r="H103" s="3" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>11/07/2025</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>30.77</v>
+      </c>
+      <c r="F104" s="2" t="inlineStr">
+        <is>
+          <t>10/58</t>
+        </is>
+      </c>
+      <c r="G104" s="2" t="n">
+        <v>114.05</v>
+      </c>
+      <c r="H104" s="2" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>11/07/2025</t>
+        </is>
+      </c>
+      <c r="C105" s="3" t="inlineStr">
+        <is>
+          <t>13/08/2025</t>
+        </is>
+      </c>
+      <c r="D105" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="E105" s="3" t="n">
+        <v>-15.69</v>
+      </c>
+      <c r="F105" s="3" t="inlineStr">
+        <is>
+          <t>25/58</t>
+        </is>
+      </c>
+      <c r="G105" s="3" t="n">
+        <v>98.37</v>
+      </c>
+      <c r="H105" s="3" t="n"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B106" s="2" t="inlineStr">
+        <is>
+          <t>13/08/2025</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
+        <is>
+          <t>15/08/2025</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="F106" s="2" t="inlineStr">
+        <is>
+          <t>43/58</t>
+        </is>
+      </c>
+      <c r="G106" s="2" t="n">
+        <v>105.17</v>
+      </c>
+      <c r="H106" s="2" t="n"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B107" s="3" t="inlineStr">
+        <is>
+          <t>15/08/2025</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
+        <is>
+          <t>21/08/2025</t>
+        </is>
+      </c>
+      <c r="D107" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E107" s="3" t="n">
+        <v>-7.64</v>
+      </c>
+      <c r="F107" s="3" t="inlineStr">
+        <is>
+          <t>44/58</t>
+        </is>
+      </c>
+      <c r="G107" s="3" t="n">
+        <v>97.53</v>
+      </c>
+      <c r="H107" s="3" t="n"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B108" s="2" t="inlineStr">
+        <is>
+          <t>21/08/2025</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="inlineStr">
+        <is>
+          <t>28/08/2025</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>7.59</v>
+      </c>
+      <c r="F108" s="2" t="inlineStr">
+        <is>
+          <t>40/58</t>
+        </is>
+      </c>
+      <c r="G108" s="2" t="n">
+        <v>105.11</v>
+      </c>
+      <c r="H108" s="2" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B109" s="3" t="inlineStr">
+        <is>
+          <t>28/08/2025</t>
+        </is>
+      </c>
+      <c r="C109" s="3" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="D109" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="E109" s="3" t="n">
+        <v>-5.13</v>
+      </c>
+      <c r="F109" s="3" t="inlineStr">
+        <is>
+          <t>49/58</t>
+        </is>
+      </c>
+      <c r="G109" s="3" t="n">
+        <v>99.98</v>
+      </c>
+      <c r="H109" s="3" t="n"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="inlineStr">
+        <is>
+          <t>06/10/2025</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="F110" s="2" t="inlineStr">
+        <is>
+          <t>51/58</t>
+        </is>
+      </c>
+      <c r="G110" s="2" t="n">
+        <v>103.36</v>
+      </c>
+      <c r="H110" s="2" t="n"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B111" s="3" t="inlineStr">
+        <is>
+          <t>06/10/2025</t>
+        </is>
+      </c>
+      <c r="C111" s="3" t="inlineStr">
+        <is>
+          <t>29/10/2025</t>
+        </is>
+      </c>
+      <c r="D111" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E111" s="3" t="n">
+        <v>-19.61</v>
+      </c>
+      <c r="F111" s="3" t="inlineStr">
+        <is>
+          <t>20/58</t>
+        </is>
+      </c>
+      <c r="G111" s="3" t="n">
+        <v>83.75</v>
+      </c>
+      <c r="H111" s="3" t="n"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B112" s="2" t="inlineStr">
+        <is>
+          <t>29/10/2025</t>
+        </is>
+      </c>
+      <c r="C112" s="2" t="inlineStr">
+        <is>
+          <t>14/11/2025</t>
+        </is>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>11.36</v>
+      </c>
+      <c r="F112" s="2" t="inlineStr">
+        <is>
+          <t>31/58</t>
+        </is>
+      </c>
+      <c r="G112" s="2" t="n">
+        <v>95.12</v>
+      </c>
+      <c r="H112" s="2" t="n"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B113" s="3" t="inlineStr">
+        <is>
+          <t>14/11/2025</t>
+        </is>
+      </c>
+      <c r="C113" s="3" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="D113" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E113" s="3" t="n">
+        <v>-16.33</v>
+      </c>
+      <c r="F113" s="3" t="inlineStr">
+        <is>
+          <t>24/58</t>
+        </is>
+      </c>
+      <c r="G113" s="3" t="n">
+        <v>78.79000000000001</v>
+      </c>
+      <c r="H113" s="3" t="n"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B114" s="2" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="C114" s="2" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="F114" s="2" t="inlineStr">
+        <is>
+          <t>41/58</t>
+        </is>
+      </c>
+      <c r="G114" s="2" t="n">
+        <v>86.11</v>
+      </c>
+      <c r="H114" s="2" t="n"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B115" s="3" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="C115" s="3" t="inlineStr">
+        <is>
           <t>31/12/2025</t>
         </is>
       </c>
-      <c r="C78" s="2" t="inlineStr">
-        <is>
-          <t>17/02/2026</t>
-        </is>
-      </c>
-      <c r="D78" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="E78" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="F78" s="2" t="inlineStr">
-        <is>
-          <t>8/39</t>
-        </is>
-      </c>
-      <c r="G78" s="2" t="n">
-        <v>203.07</v>
-      </c>
-      <c r="H78" s="2" t="inlineStr"/>
+      <c r="D115" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E115" s="3" t="n">
+        <v>-16.67</v>
+      </c>
+      <c r="F115" s="3" t="inlineStr">
+        <is>
+          <t>23/58</t>
+        </is>
+      </c>
+      <c r="G115" s="3" t="n">
+        <v>69.44</v>
+      </c>
+      <c r="H115" s="3" t="n"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B116" s="2" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C116" s="2" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="D116" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>39.09</v>
+      </c>
+      <c r="F116" s="2" t="inlineStr">
+        <is>
+          <t>7/58</t>
+        </is>
+      </c>
+      <c r="G116" s="2" t="n">
+        <v>108.53</v>
+      </c>
+      <c r="H116" s="2" t="n"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B117" s="3" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="C117" s="3" t="inlineStr">
+        <is>
+          <t>11/02/2026</t>
+        </is>
+      </c>
+      <c r="D117" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E117" s="3" t="n">
+        <v>-3.27</v>
+      </c>
+      <c r="F117" s="3" t="inlineStr">
+        <is>
+          <t>52/58</t>
+        </is>
+      </c>
+      <c r="G117" s="3" t="n">
+        <v>105.26</v>
+      </c>
+      <c r="H117" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refine insider strategy; improve XLSX output formatting
Enhanced insider conviction strategy logic and updated XLSX output for Grov rise events, ensuring better readability and accuracy.

Key changes:
- Adjusted rise detection logic to account for hot stock scenarios.
- Added plateau detection for minimal price movements.
- Improved XLSX formatting for Grov rise events.
- Removed temporary XLSX file from output directory.

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/grov_rise_events.xlsx
+++ b/output CSVs/grov_rise_events.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,24 +510,28 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>10/06/2021</t>
+          <t>20/06/2022</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2</v>
+        <v>377</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>1.23</v>
+        <v>2.25</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>57/58</t>
+          <t>40/40</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="H2" s="2" t="n"/>
+        <v>2.25</v>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>16/06/2022</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -537,27 +541,27 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>10/06/2021</t>
+          <t>21/06/2022</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>29/06/2021</t>
+          <t>20/07/2022</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>-1.31</v>
+        <v>-60</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>54/58</t>
+          <t>3/40</t>
         </is>
       </c>
       <c r="G3" s="3" t="n">
-        <v>-0.09</v>
+        <v>-57.75</v>
       </c>
       <c r="H3" s="3" t="n"/>
     </row>
@@ -569,27 +573,27 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>29/06/2021</t>
+          <t>20/07/2022</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>05/08/2021</t>
+          <t>01/08/2022</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.41</v>
+        <v>4.91</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>58/58</t>
+          <t>37/40</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>0.32</v>
+        <v>-52.84</v>
       </c>
       <c r="H4" s="2" t="n"/>
     </row>
@@ -601,27 +605,27 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>05/08/2021</t>
+          <t>02/08/2022</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>07/09/2021</t>
+          <t>08/08/2022</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>-1.63</v>
+        <v>-12.13</v>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>53/58</t>
+          <t>29/40</t>
         </is>
       </c>
       <c r="G5" s="3" t="n">
-        <v>-1.31</v>
+        <v>-64.97</v>
       </c>
       <c r="H5" s="3" t="n"/>
     </row>
@@ -633,27 +637,27 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>07/09/2021</t>
+          <t>08/08/2022</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>04/11/2021</t>
+          <t>18/08/2022</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1.86</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>54/58</t>
+          <t>3/40</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>0.55</v>
+        <v>4.04</v>
       </c>
       <c r="H6" s="2" t="n"/>
     </row>
@@ -665,29 +669,33 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>04/11/2021</t>
+          <t>19/08/2022</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>06/12/2021</t>
+          <t>01/09/2022</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>-0.91</v>
+        <v>-32.66</v>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>56/58</t>
+          <t>7/40</t>
         </is>
       </c>
       <c r="G7" s="3" t="n">
-        <v>-0.36</v>
-      </c>
-      <c r="H7" s="3" t="n"/>
+        <v>-28.62</v>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>30/08/2022</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -697,27 +705,27 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>06/12/2021</t>
+          <t>01/09/2022</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>05/01/2022</t>
+          <t>16/09/2022</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>1.53</v>
+        <v>44.19</v>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>55/58</t>
+          <t>7/40</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
-        <v>1.17</v>
+        <v>15.57</v>
       </c>
       <c r="H8" s="2" t="n"/>
     </row>
@@ -729,27 +737,27 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>05/01/2022</t>
+          <t>19/09/2022</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>19/01/2022</t>
+          <t>03/10/2022</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
         <v>14</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>-1.11</v>
+        <v>-68.06</v>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>55/58</t>
+          <t>2/40</t>
         </is>
       </c>
       <c r="G9" s="3" t="n">
-        <v>0.06</v>
+        <v>-52.49</v>
       </c>
       <c r="H9" s="3" t="n"/>
     </row>
@@ -761,27 +769,27 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>19/01/2022</t>
+          <t>03/10/2022</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>06/06/2022</t>
+          <t>19/10/2022</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>137</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>1.32</v>
+        <v>4.95</v>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>56/58</t>
+          <t>36/40</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>1.39</v>
+        <v>-47.54</v>
       </c>
       <c r="H10" s="2" t="n"/>
     </row>
@@ -793,27 +801,27 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>06/06/2022</t>
+          <t>20/10/2022</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>20/07/2022</t>
+          <t>03/11/2022</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>-59.84</v>
+        <v>-54.08</v>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>3/58</t>
+          <t>5/40</t>
         </is>
       </c>
       <c r="G11" s="3" t="n">
-        <v>-58.45</v>
+        <v>-101.61</v>
       </c>
       <c r="H11" s="3" t="n"/>
     </row>
@@ -825,27 +833,27 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>20/07/2022</t>
+          <t>03/11/2022</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>01/08/2022</t>
+          <t>09/11/2022</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>4.91</v>
+        <v>17.76</v>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>47/58</t>
+          <t>20/40</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
-        <v>-53.54</v>
+        <v>-83.86</v>
       </c>
       <c r="H12" s="2" t="n"/>
     </row>
@@ -857,29 +865,33 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>01/08/2022</t>
+          <t>10/11/2022</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>08/08/2022</t>
+          <t>20/12/2022</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>-12.13</v>
+        <v>-83.73</v>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>31/58</t>
+          <t>1/40</t>
         </is>
       </c>
       <c r="G13" s="3" t="n">
-        <v>-65.67</v>
-      </c>
-      <c r="H13" s="3" t="n"/>
+        <v>-167.59</v>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>22/11/2022, 05/12/2022</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
@@ -889,27 +901,27 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>08/08/2022</t>
+          <t>20/12/2022</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>18/08/2022</t>
+          <t>17/01/2023</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>69.01000000000001</v>
+        <v>197.56</v>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>3/58</t>
+          <t>1/40</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
-        <v>3.34</v>
+        <v>29.97</v>
       </c>
       <c r="H14" s="2" t="n"/>
     </row>
@@ -921,33 +933,29 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>18/08/2022</t>
+          <t>18/01/2023</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>01/09/2022</t>
+          <t>30/01/2023</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>-32.66</v>
+        <v>-29.51</v>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>7/58</t>
+          <t>9/40</t>
         </is>
       </c>
       <c r="G15" s="3" t="n">
-        <v>-29.33</v>
-      </c>
-      <c r="H15" s="3" t="inlineStr">
-        <is>
-          <t>30/08/2022</t>
-        </is>
-      </c>
+        <v>0.47</v>
+      </c>
+      <c r="H15" s="3" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
@@ -957,27 +965,27 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>01/09/2022</t>
+          <t>30/01/2023</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>16/09/2022</t>
+          <t>06/02/2023</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>44.19</v>
+        <v>21.86</v>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>6/58</t>
+          <t>17/40</t>
         </is>
       </c>
       <c r="G16" s="2" t="n">
-        <v>14.86</v>
+        <v>22.33</v>
       </c>
       <c r="H16" s="2" t="n"/>
     </row>
@@ -989,27 +997,27 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>16/09/2022</t>
+          <t>07/02/2023</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>03/10/2022</t>
+          <t>01/03/2023</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>-68.06</v>
+        <v>-23.47</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>2/58</t>
+          <t>17/40</t>
         </is>
       </c>
       <c r="G17" s="3" t="n">
-        <v>-53.2</v>
+        <v>-1.15</v>
       </c>
       <c r="H17" s="3" t="n"/>
     </row>
@@ -1021,27 +1029,27 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>03/10/2022</t>
+          <t>01/03/2023</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>05/10/2022</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>4.95</v>
+        <v>29.93</v>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>46/58</t>
+          <t>11/40</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>-48.24</v>
+        <v>28.78</v>
       </c>
       <c r="H18" s="2" t="n"/>
     </row>
@@ -1053,29 +1061,33 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>05/10/2022</t>
+          <t>08/03/2023</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>03/11/2022</t>
+          <t>20/03/2023</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>-54.08</v>
+        <v>-41.07</v>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>4/58</t>
+          <t>6/40</t>
         </is>
       </c>
       <c r="G19" s="3" t="n">
-        <v>-102.32</v>
-      </c>
-      <c r="H19" s="3" t="n"/>
+        <v>-12.29</v>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>17/03/2023</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
@@ -1085,27 +1097,27 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>03/11/2022</t>
+          <t>20/03/2023</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>09/11/2022</t>
+          <t>04/04/2023</t>
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>17.76</v>
+        <v>52.42</v>
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>21/58</t>
+          <t>4/40</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
-        <v>-84.56</v>
+        <v>40.14</v>
       </c>
       <c r="H20" s="2" t="n"/>
     </row>
@@ -1117,33 +1129,29 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>09/11/2022</t>
+          <t>05/04/2023</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>20/12/2022</t>
+          <t>13/04/2023</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>-83.73</v>
+        <v>-11.73</v>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>1/58</t>
+          <t>30/40</t>
         </is>
       </c>
       <c r="G21" s="3" t="n">
-        <v>-168.29</v>
-      </c>
-      <c r="H21" s="3" t="inlineStr">
-        <is>
-          <t>22/11/2022, 05/12/2022</t>
-        </is>
-      </c>
+        <v>28.41</v>
+      </c>
+      <c r="H21" s="3" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
@@ -1153,27 +1161,27 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>20/12/2022</t>
+          <t>13/04/2023</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>17/01/2023</t>
+          <t>19/04/2023</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>197.56</v>
+        <v>11.56</v>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>1/58</t>
+          <t>24/40</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
-        <v>29.27</v>
+        <v>39.96</v>
       </c>
       <c r="H22" s="2" t="n"/>
     </row>
@@ -1185,27 +1193,27 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>17/01/2023</t>
+          <t>20/04/2023</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>30/01/2023</t>
+          <t>26/04/2023</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>-29.51</v>
+        <v>-10.36</v>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>9/58</t>
+          <t>32/40</t>
         </is>
       </c>
       <c r="G23" s="3" t="n">
-        <v>-0.24</v>
+        <v>29.6</v>
       </c>
       <c r="H23" s="3" t="n"/>
     </row>
@@ -1217,27 +1225,27 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>30/01/2023</t>
+          <t>26/04/2023</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>06/02/2023</t>
+          <t>28/04/2023</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>21.86</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>15/58</t>
+          <t>28/40</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
-        <v>21.62</v>
+        <v>38.49</v>
       </c>
       <c r="H24" s="2" t="n"/>
     </row>
@@ -1249,29 +1257,33 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>06/02/2023</t>
+          <t>01/05/2023</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>01/03/2023</t>
+          <t>09/06/2023</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>-23.47</v>
+        <v>-26.94</v>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>16/58</t>
+          <t>12/40</t>
         </is>
       </c>
       <c r="G25" s="3" t="n">
-        <v>-1.85</v>
-      </c>
-      <c r="H25" s="3" t="n"/>
+        <v>11.55</v>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>17/05/2023, 22/05/2023, 23/05/2023, 24/05/2023, 26/05/2023, 30/05/2023, 01/06/2023</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
@@ -1281,27 +1293,27 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>01/03/2023</t>
+          <t>09/06/2023</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>07/03/2023</t>
+          <t>14/06/2023</t>
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>29.93</v>
+        <v>18.44</v>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>12/58</t>
+          <t>18/40</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>28.08</v>
+        <v>29.99</v>
       </c>
       <c r="H26" s="2" t="n"/>
     </row>
@@ -1313,33 +1325,29 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>07/03/2023</t>
+          <t>15/06/2023</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>20/03/2023</t>
+          <t>03/07/2023</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>-41.07</v>
+        <v>-22.64</v>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>6/58</t>
+          <t>18/40</t>
         </is>
       </c>
       <c r="G27" s="3" t="n">
-        <v>-12.99</v>
-      </c>
-      <c r="H27" s="3" t="inlineStr">
-        <is>
-          <t>17/03/2023</t>
-        </is>
-      </c>
+        <v>7.35</v>
+      </c>
+      <c r="H27" s="3" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
@@ -1349,27 +1357,27 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>20/03/2023</t>
+          <t>03/07/2023</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>04/04/2023</t>
+          <t>21/07/2023</t>
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>52.42</v>
+        <v>23.03</v>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>4/58</t>
+          <t>15/40</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>39.43</v>
+        <v>30.38</v>
       </c>
       <c r="H28" s="2" t="n"/>
     </row>
@@ -1381,27 +1389,27 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>04/04/2023</t>
+          <t>24/07/2023</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>13/04/2023</t>
+          <t>03/08/2023</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>-11.73</v>
+        <v>-15.53</v>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>33/58</t>
+          <t>24/40</t>
         </is>
       </c>
       <c r="G29" s="3" t="n">
-        <v>27.7</v>
+        <v>14.86</v>
       </c>
       <c r="H29" s="3" t="n"/>
     </row>
@@ -1413,27 +1421,27 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>13/04/2023</t>
+          <t>03/08/2023</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>18/04/2023</t>
+          <t>28/09/2023</t>
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>11.56</v>
+        <v>87.95999999999999</v>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>30/58</t>
+          <t>2/40</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>39.26</v>
+        <v>102.81</v>
       </c>
       <c r="H30" s="2" t="n"/>
     </row>
@@ -1445,27 +1453,27 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>18/04/2023</t>
+          <t>29/09/2023</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>26/04/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="D31" s="3" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>-10.36</v>
+        <v>-54.87</v>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>37/58</t>
+          <t>4/40</t>
         </is>
       </c>
       <c r="G31" s="3" t="n">
-        <v>28.9</v>
+        <v>47.94</v>
       </c>
       <c r="H31" s="3" t="n"/>
     </row>
@@ -1477,27 +1485,27 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>26/04/2023</t>
+          <t>13/10/2023</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>28/04/2023</t>
+          <t>19/10/2023</t>
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>8.890000000000001</v>
+        <v>16.67</v>
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>36/58</t>
+          <t>21/40</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
-        <v>37.79</v>
+        <v>64.61</v>
       </c>
       <c r="H32" s="2" t="n"/>
     </row>
@@ -1509,33 +1517,29 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>28/04/2023</t>
+          <t>20/10/2023</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>09/06/2023</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="D33" s="3" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>-26.94</v>
+        <v>-19.58</v>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>11/58</t>
+          <t>22/40</t>
         </is>
       </c>
       <c r="G33" s="3" t="n">
-        <v>10.85</v>
-      </c>
-      <c r="H33" s="3" t="inlineStr">
-        <is>
-          <t>17/05/2023, 22/05/2023, 23/05/2023, 24/05/2023, 26/05/2023, 30/05/2023, 01/06/2023</t>
-        </is>
-      </c>
+        <v>45.03</v>
+      </c>
+      <c r="H33" s="3" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
@@ -1545,27 +1549,27 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>09/06/2023</t>
+          <t>03/11/2023</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>13/06/2023</t>
+          <t>23/11/2023</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>18.44</v>
+        <v>50</v>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>18/58</t>
+          <t>5/40</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>29.29</v>
+        <v>95.03</v>
       </c>
       <c r="H34" s="2" t="n"/>
     </row>
@@ -1577,27 +1581,27 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>13/06/2023</t>
+          <t>24/11/2023</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>12/12/2023</t>
         </is>
       </c>
       <c r="D35" s="3" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E35" s="3" t="n">
-        <v>-22.64</v>
+        <v>-27.35</v>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>17/58</t>
+          <t>11/40</t>
         </is>
       </c>
       <c r="G35" s="3" t="n">
-        <v>6.64</v>
+        <v>67.68000000000001</v>
       </c>
       <c r="H35" s="3" t="n"/>
     </row>
@@ -1609,29 +1613,33 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>12/12/2023</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>33.54</v>
+        <v>24.71</v>
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>9/58</t>
+          <t>13/40</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>40.18</v>
-      </c>
-      <c r="H36" s="2" t="n"/>
+        <v>92.39</v>
+      </c>
+      <c r="H36" s="2" t="inlineStr">
+        <is>
+          <t>14/12/2023</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
@@ -1641,27 +1649,27 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>03/08/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="D37" s="3" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>-15.53</v>
+        <v>-22.17</v>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>26/58</t>
+          <t>19/40</t>
         </is>
       </c>
       <c r="G37" s="3" t="n">
-        <v>24.66</v>
+        <v>70.22</v>
       </c>
       <c r="H37" s="3" t="n"/>
     </row>
@@ -1673,27 +1681,27 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>03/08/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>18/08/2023</t>
+          <t>12/02/2024</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>78.01000000000001</v>
+        <v>10.3</v>
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>2/58</t>
+          <t>25/40</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>102.67</v>
+        <v>80.52</v>
       </c>
       <c r="H38" s="2" t="n"/>
     </row>
@@ -1705,27 +1713,27 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>18/08/2023</t>
+          <t>13/02/2024</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>24/08/2023</t>
+          <t>22/02/2024</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>-8.529999999999999</v>
+        <v>-8.789999999999999</v>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>43/58</t>
+          <t>34/40</t>
         </is>
       </c>
       <c r="G39" s="3" t="n">
-        <v>94.14</v>
+        <v>71.73</v>
       </c>
       <c r="H39" s="3" t="n"/>
     </row>
@@ -1737,29 +1745,33 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>24/08/2023</t>
+          <t>22/02/2024</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>29/08/2023</t>
+          <t>15/03/2024</t>
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>15.43</v>
+        <v>36.9</v>
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>24/58</t>
+          <t>9/40</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>109.57</v>
-      </c>
-      <c r="H40" s="2" t="n"/>
+        <v>108.63</v>
+      </c>
+      <c r="H40" s="2" t="inlineStr">
+        <is>
+          <t>08/03/2024, 11/03/2024</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
@@ -1769,27 +1781,27 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>29/08/2023</t>
+          <t>18/03/2024</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>13/09/2023</t>
+          <t>03/04/2024</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>-23.96</v>
+        <v>-32.61</v>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>15/58</t>
+          <t>8/40</t>
         </is>
       </c>
       <c r="G41" s="3" t="n">
-        <v>85.62</v>
+        <v>76.02</v>
       </c>
       <c r="H41" s="3" t="n"/>
     </row>
@@ -1801,27 +1813,27 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>13/09/2023</t>
+          <t>03/04/2024</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>15/09/2023</t>
+          <t>08/04/2024</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>17.22</v>
+        <v>9.68</v>
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>22/58</t>
+          <t>26/40</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>102.83</v>
+        <v>85.7</v>
       </c>
       <c r="H42" s="2" t="n"/>
     </row>
@@ -1833,27 +1845,27 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>15/09/2023</t>
+          <t>09/04/2024</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>13/10/2023</t>
+          <t>17/04/2024</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>-49.38</v>
+        <v>-15.29</v>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>5/58</t>
+          <t>25/40</t>
         </is>
       </c>
       <c r="G43" s="3" t="n">
-        <v>53.46</v>
+        <v>70.41</v>
       </c>
       <c r="H43" s="3" t="n"/>
     </row>
@@ -1865,27 +1877,27 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>13/10/2023</t>
+          <t>17/04/2024</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>19/10/2023</t>
+          <t>22/04/2024</t>
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>16.67</v>
+        <v>7.89</v>
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>23/58</t>
+          <t>30/40</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>70.12</v>
+        <v>78.3</v>
       </c>
       <c r="H44" s="2" t="n"/>
     </row>
@@ -1897,27 +1909,27 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>19/10/2023</t>
+          <t>23/04/2024</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>03/11/2023</t>
+          <t>30/04/2024</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>-19.58</v>
+        <v>-8.539999999999999</v>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>21/58</t>
+          <t>35/40</t>
         </is>
       </c>
       <c r="G45" s="3" t="n">
-        <v>50.55</v>
+        <v>69.76000000000001</v>
       </c>
       <c r="H45" s="3" t="n"/>
     </row>
@@ -1929,27 +1941,27 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>03/11/2023</t>
+          <t>30/04/2024</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>22/11/2023</t>
+          <t>09/05/2024</t>
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>5/58</t>
+          <t>22/40</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
-        <v>100.55</v>
+        <v>83.76000000000001</v>
       </c>
       <c r="H46" s="2" t="n"/>
     </row>
@@ -1961,27 +1973,27 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>22/11/2023</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>12/12/2023</t>
+          <t>16/05/2024</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>-27.35</v>
+        <v>-12.87</v>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>10/58</t>
+          <t>27/40</t>
         </is>
       </c>
       <c r="G47" s="3" t="n">
-        <v>73.2</v>
+        <v>70.90000000000001</v>
       </c>
       <c r="H47" s="3" t="n"/>
     </row>
@@ -1993,31 +2005,31 @@
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>12/12/2023</t>
+          <t>16/05/2024</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>14/12/2023</t>
+          <t>04/07/2024</t>
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>12.35</v>
+        <v>23.49</v>
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>28/58</t>
+          <t>14/40</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>85.55</v>
+        <v>94.39</v>
       </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
-          <t>14/12/2023</t>
+          <t>29/05/2024</t>
         </is>
       </c>
     </row>
@@ -2029,27 +2041,27 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>14/12/2023</t>
+          <t>05/07/2024</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>06/08/2024</t>
         </is>
       </c>
       <c r="D49" s="3" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>-4.71</v>
+        <v>-26.63</v>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>50/58</t>
+          <t>13/40</t>
         </is>
       </c>
       <c r="G49" s="3" t="n">
-        <v>80.84</v>
+        <v>67.76000000000001</v>
       </c>
       <c r="H49" s="3" t="n"/>
     </row>
@@ -2061,27 +2073,27 @@
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>06/08/2024</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>22/12/2023</t>
+          <t>08/08/2024</t>
         </is>
       </c>
       <c r="D50" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>9.890000000000001</v>
+        <v>5.15</v>
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>33/58</t>
+          <t>35/40</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>90.73</v>
+        <v>72.91</v>
       </c>
       <c r="H50" s="2" t="n"/>
     </row>
@@ -2093,27 +2105,27 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>22/12/2023</t>
+          <t>09/08/2024</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>29/12/2023</t>
+          <t>14/08/2024</t>
         </is>
       </c>
       <c r="D51" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>-11.5</v>
+        <v>-11.19</v>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>35/58</t>
+          <t>31/40</t>
         </is>
       </c>
       <c r="G51" s="3" t="n">
-        <v>79.23</v>
+        <v>61.72</v>
       </c>
       <c r="H51" s="3" t="n"/>
     </row>
@@ -2125,27 +2137,27 @@
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>29/12/2023</t>
+          <t>14/08/2024</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>19.77</v>
+        <v>7.09</v>
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>16/58</t>
+          <t>31/40</t>
         </is>
       </c>
       <c r="G52" s="2" t="n">
-        <v>99</v>
+        <v>68.8</v>
       </c>
       <c r="H52" s="2" t="n"/>
     </row>
@@ -2157,27 +2169,27 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>19/08/2024</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>26/01/2024</t>
+          <t>11/09/2024</t>
         </is>
       </c>
       <c r="D53" s="3" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>-19.81</v>
+        <v>-6.62</v>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>19/58</t>
+          <t>36/40</t>
         </is>
       </c>
       <c r="G53" s="3" t="n">
-        <v>79.19</v>
+        <v>62.19</v>
       </c>
       <c r="H53" s="3" t="n"/>
     </row>
@@ -2189,27 +2201,27 @@
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>26/01/2024</t>
+          <t>11/09/2024</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>31/01/2024</t>
+          <t>19/09/2024</t>
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>7.65</v>
+        <v>9.02</v>
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>39/58</t>
+          <t>27/40</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
-        <v>86.84</v>
+        <v>71.20999999999999</v>
       </c>
       <c r="H54" s="2" t="n"/>
     </row>
@@ -2221,27 +2233,27 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>31/01/2024</t>
+          <t>20/09/2024</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>07/11/2024</t>
         </is>
       </c>
       <c r="D55" s="3" t="n">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>-9.84</v>
+        <v>-13.1</v>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>38/58</t>
+          <t>26/40</t>
         </is>
       </c>
       <c r="G55" s="3" t="n">
-        <v>77</v>
+        <v>58.11</v>
       </c>
       <c r="H55" s="3" t="n"/>
     </row>
@@ -2253,29 +2265,33 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>07/11/2024</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>08/02/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>10.3</v>
+        <v>18.32</v>
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>32/58</t>
+          <t>19/40</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
-        <v>87.3</v>
-      </c>
-      <c r="H56" s="2" t="n"/>
+        <v>76.43000000000001</v>
+      </c>
+      <c r="H56" s="2" t="inlineStr">
+        <is>
+          <t>18/11/2024</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
@@ -2285,27 +2301,27 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>08/02/2024</t>
+          <t>03/12/2024</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>22/02/2024</t>
+          <t>31/12/2024</t>
         </is>
       </c>
       <c r="D57" s="3" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>-8.789999999999999</v>
+        <v>-12.26</v>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>41/58</t>
+          <t>28/40</t>
         </is>
       </c>
       <c r="G57" s="3" t="n">
-        <v>78.51000000000001</v>
+        <v>64.17</v>
       </c>
       <c r="H57" s="3" t="n"/>
     </row>
@@ -2317,27 +2333,27 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>22/02/2024</t>
+          <t>31/12/2024</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>05/03/2024</t>
+          <t>09/01/2025</t>
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>36.9</v>
+        <v>26.62</v>
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>8/58</t>
+          <t>12/40</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
-        <v>115.42</v>
+        <v>90.79000000000001</v>
       </c>
       <c r="H58" s="2" t="n"/>
     </row>
@@ -2349,27 +2365,27 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>05/03/2024</t>
+          <t>10/01/2025</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>03/04/2024</t>
+          <t>30/01/2025</t>
         </is>
       </c>
       <c r="D59" s="3" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>-32.61</v>
+        <v>-24.43</v>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>8/58</t>
+          <t>16/40</t>
         </is>
       </c>
       <c r="G59" s="3" t="n">
-        <v>82.81</v>
+        <v>66.34999999999999</v>
       </c>
       <c r="H59" s="3" t="n"/>
     </row>
@@ -2381,27 +2397,27 @@
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>03/04/2024</t>
+          <t>30/01/2025</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>08/04/2024</t>
+          <t>05/02/2025</t>
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>9.68</v>
+        <v>23.02</v>
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>34/58</t>
+          <t>16/40</t>
         </is>
       </c>
       <c r="G60" s="2" t="n">
-        <v>92.48999999999999</v>
+        <v>89.38</v>
       </c>
       <c r="H60" s="2" t="n"/>
     </row>
@@ -2413,27 +2429,27 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>08/04/2024</t>
+          <t>06/02/2025</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>17/04/2024</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="D61" s="3" t="n">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>-15.29</v>
+        <v>-21.64</v>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>27/58</t>
+          <t>20/40</t>
         </is>
       </c>
       <c r="G61" s="3" t="n">
-        <v>77.19</v>
+        <v>67.73999999999999</v>
       </c>
       <c r="H61" s="3" t="n"/>
     </row>
@@ -2445,27 +2461,27 @@
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>17/04/2024</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>22/04/2024</t>
+          <t>03/04/2025</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>7.89</v>
+        <v>3.73</v>
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>38/58</t>
+          <t>38/40</t>
         </is>
       </c>
       <c r="G62" s="2" t="n">
-        <v>85.09</v>
+        <v>71.47</v>
       </c>
       <c r="H62" s="2" t="n"/>
     </row>
@@ -2477,27 +2493,27 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>22/04/2024</t>
+          <t>04/04/2025</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>30/04/2024</t>
+          <t>11/04/2025</t>
         </is>
       </c>
       <c r="D63" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>-8.539999999999999</v>
+        <v>-24.46</v>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>42/58</t>
+          <t>15/40</t>
         </is>
       </c>
       <c r="G63" s="3" t="n">
-        <v>76.55</v>
+        <v>47.01</v>
       </c>
       <c r="H63" s="3" t="n"/>
     </row>
@@ -2509,27 +2525,27 @@
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>30/04/2024</t>
+          <t>11/04/2025</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>09/05/2024</t>
+          <t>15/04/2025</t>
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>14</v>
+        <v>6.67</v>
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>26/58</t>
+          <t>33/40</t>
         </is>
       </c>
       <c r="G64" s="2" t="n">
-        <v>90.55</v>
+        <v>53.68</v>
       </c>
       <c r="H64" s="2" t="n"/>
     </row>
@@ -2541,27 +2557,27 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>09/05/2024</t>
+          <t>16/04/2025</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>16/05/2024</t>
+          <t>22/04/2025</t>
         </is>
       </c>
       <c r="D65" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>-12.87</v>
+        <v>-6.25</v>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>29/58</t>
+          <t>37/40</t>
         </is>
       </c>
       <c r="G65" s="3" t="n">
-        <v>77.68000000000001</v>
+        <v>47.43</v>
       </c>
       <c r="H65" s="3" t="n"/>
     </row>
@@ -2573,33 +2589,29 @@
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>16/05/2024</t>
+          <t>22/04/2025</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>14/06/2024</t>
+          <t>29/04/2025</t>
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>18.12</v>
+        <v>8.57</v>
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>20/58</t>
+          <t>29/40</t>
         </is>
       </c>
       <c r="G66" s="2" t="n">
-        <v>95.81</v>
-      </c>
-      <c r="H66" s="2" t="inlineStr">
-        <is>
-          <t>29/05/2024</t>
-        </is>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H66" s="2" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
@@ -2609,27 +2621,27 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>14/06/2024</t>
+          <t>30/04/2025</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>25/06/2024</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="D67" s="3" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>-9.09</v>
+        <v>-5.26</v>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>40/58</t>
+          <t>39/40</t>
         </is>
       </c>
       <c r="G67" s="3" t="n">
-        <v>86.70999999999999</v>
+        <v>50.73</v>
       </c>
       <c r="H67" s="3" t="n"/>
     </row>
@@ -2641,27 +2653,27 @@
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>25/06/2024</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>03/07/2024</t>
+          <t>12/05/2025</t>
         </is>
       </c>
       <c r="D68" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>15</v>
+        <v>12.96</v>
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>25/58</t>
+          <t>23/40</t>
         </is>
       </c>
       <c r="G68" s="2" t="n">
-        <v>101.71</v>
+        <v>63.7</v>
       </c>
       <c r="H68" s="2" t="n"/>
     </row>
@@ -2673,27 +2685,27 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>03/07/2024</t>
+          <t>13/05/2025</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>05/08/2024</t>
+          <t>19/05/2025</t>
         </is>
       </c>
       <c r="D69" s="3" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>-26.63</v>
+        <v>-9.84</v>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>12/58</t>
+          <t>33/40</t>
         </is>
       </c>
       <c r="G69" s="3" t="n">
-        <v>75.08</v>
+        <v>53.86</v>
       </c>
       <c r="H69" s="3" t="n"/>
     </row>
@@ -2705,29 +2717,33 @@
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>05/08/2024</t>
+          <t>19/05/2025</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>08/08/2024</t>
+          <t>27/05/2025</t>
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>5.93</v>
+        <v>30</v>
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>45/58</t>
+          <t>10/40</t>
         </is>
       </c>
       <c r="G70" s="2" t="n">
-        <v>81.01000000000001</v>
-      </c>
-      <c r="H70" s="2" t="n"/>
+        <v>83.86</v>
+      </c>
+      <c r="H70" s="2" t="inlineStr">
+        <is>
+          <t>23/05/2025, 27/05/2025</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
@@ -2737,29 +2753,33 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>08/08/2024</t>
+          <t>28/05/2025</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>14/08/2024</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="D71" s="3" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>-11.19</v>
+        <v>-27.97</v>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>36/58</t>
+          <t>10/40</t>
         </is>
       </c>
       <c r="G71" s="3" t="n">
-        <v>69.81999999999999</v>
-      </c>
-      <c r="H71" s="3" t="n"/>
+        <v>55.89</v>
+      </c>
+      <c r="H71" s="3" t="inlineStr">
+        <is>
+          <t>02/06/2025, 06/06/2025, 09/06/2025, 10/06/2025, 12/06/2025, 13/06/2025</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
@@ -2769,27 +2789,27 @@
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>14/08/2024</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>16/08/2024</t>
+          <t>11/07/2025</t>
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>7.09</v>
+        <v>48.54</v>
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>42/58</t>
+          <t>6/40</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
-        <v>76.91</v>
+        <v>104.43</v>
       </c>
       <c r="H72" s="2" t="n"/>
     </row>
@@ -2801,27 +2821,27 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>16/08/2024</t>
+          <t>14/07/2025</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>13/08/2025</t>
         </is>
       </c>
       <c r="D73" s="3" t="n">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E73" s="3" t="n">
-        <v>-6.62</v>
+        <v>-15.69</v>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>45/58</t>
+          <t>23/40</t>
         </is>
       </c>
       <c r="G73" s="3" t="n">
-        <v>70.29000000000001</v>
+        <v>88.75</v>
       </c>
       <c r="H73" s="3" t="n"/>
     </row>
@@ -2833,27 +2853,27 @@
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>13/08/2025</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>04/09/2024</t>
+          <t>25/08/2025</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>3.88</v>
+        <v>6.8</v>
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>49/58</t>
+          <t>32/40</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
-        <v>74.17</v>
+        <v>95.55</v>
       </c>
       <c r="H74" s="2" t="n"/>
     </row>
@@ -2865,27 +2885,27 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>04/09/2024</t>
+          <t>26/08/2025</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>11/09/2024</t>
+          <t>29/09/2025</t>
         </is>
       </c>
       <c r="D75" s="3" t="n">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E75" s="3" t="n">
-        <v>-0.75</v>
+        <v>-5.73</v>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>58/58</t>
+          <t>38/40</t>
         </is>
       </c>
       <c r="G75" s="3" t="n">
-        <v>73.42</v>
+        <v>89.81999999999999</v>
       </c>
       <c r="H75" s="3" t="n"/>
     </row>
@@ -2897,27 +2917,27 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>11/09/2024</t>
+          <t>29/09/2025</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>06/10/2025</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>9.02</v>
+        <v>3.38</v>
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>35/58</t>
+          <t>39/40</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
-        <v>82.44</v>
+        <v>93.2</v>
       </c>
       <c r="H76" s="2" t="n"/>
     </row>
@@ -2929,27 +2949,27 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>07/10/2025</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>10/11/2025</t>
         </is>
       </c>
       <c r="D77" s="3" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>-11.72</v>
+        <v>-19.61</v>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>34/58</t>
+          <t>21/40</t>
         </is>
       </c>
       <c r="G77" s="3" t="n">
-        <v>70.72</v>
+        <v>73.59</v>
       </c>
       <c r="H77" s="3" t="n"/>
     </row>
@@ -2961,27 +2981,27 @@
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>10/11/2025</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>14/11/2025</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
         <v>4</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>3.13</v>
+        <v>6.52</v>
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>52/58</t>
+          <t>34/40</t>
         </is>
       </c>
       <c r="G78" s="2" t="n">
-        <v>73.84</v>
+        <v>80.11</v>
       </c>
       <c r="H78" s="2" t="n"/>
     </row>
@@ -2993,27 +3013,27 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>31/12/2025</t>
         </is>
       </c>
       <c r="D79" s="3" t="n">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E79" s="3" t="n">
-        <v>-4.55</v>
+        <v>-25.17</v>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>51/58</t>
+          <t>14/40</t>
         </is>
       </c>
       <c r="G79" s="3" t="n">
-        <v>69.3</v>
+        <v>54.94</v>
       </c>
       <c r="H79" s="3" t="n"/>
     </row>
@@ -3025,27 +3045,27 @@
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>31/12/2025</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>03/02/2026</t>
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>18.75</v>
+        <v>39.09</v>
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>17/58</t>
+          <t>8/40</t>
         </is>
       </c>
       <c r="G80" s="2" t="n">
-        <v>88.05</v>
+        <v>94.03</v>
       </c>
       <c r="H80" s="2" t="n"/>
     </row>
@@ -3057,1189 +3077,29 @@
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>04/02/2026</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>26/11/2024</t>
+          <t>11/02/2026</t>
         </is>
       </c>
       <c r="D81" s="3" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E81" s="3" t="n">
-        <v>-13.82</v>
+        <v>-3.27</v>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>28/58</t>
+          <t>40/40</t>
         </is>
       </c>
       <c r="G81" s="3" t="n">
-        <v>74.23</v>
+        <v>90.76000000000001</v>
       </c>
       <c r="H81" s="3" t="n"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B82" s="2" t="inlineStr">
-        <is>
-          <t>26/11/2024</t>
-        </is>
-      </c>
-      <c r="C82" s="2" t="inlineStr">
-        <is>
-          <t>29/11/2024</t>
-        </is>
-      </c>
-      <c r="D82" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E82" s="2" t="n">
-        <v>18.32</v>
-      </c>
-      <c r="F82" s="2" t="inlineStr">
-        <is>
-          <t>19/58</t>
-        </is>
-      </c>
-      <c r="G82" s="2" t="n">
-        <v>92.55</v>
-      </c>
-      <c r="H82" s="2" t="n"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B83" s="3" t="inlineStr">
-        <is>
-          <t>29/11/2024</t>
-        </is>
-      </c>
-      <c r="C83" s="3" t="inlineStr">
-        <is>
-          <t>23/12/2024</t>
-        </is>
-      </c>
-      <c r="D83" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E83" s="3" t="n">
-        <v>-12.26</v>
-      </c>
-      <c r="F83" s="3" t="inlineStr">
-        <is>
-          <t>30/58</t>
-        </is>
-      </c>
-      <c r="G83" s="3" t="n">
-        <v>80.29000000000001</v>
-      </c>
-      <c r="H83" s="3" t="n"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B84" s="2" t="inlineStr">
-        <is>
-          <t>23/12/2024</t>
-        </is>
-      </c>
-      <c r="C84" s="2" t="inlineStr">
-        <is>
-          <t>08/01/2025</t>
-        </is>
-      </c>
-      <c r="D84" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="E84" s="2" t="n">
-        <v>29.41</v>
-      </c>
-      <c r="F84" s="2" t="inlineStr">
-        <is>
-          <t>13/58</t>
-        </is>
-      </c>
-      <c r="G84" s="2" t="n">
-        <v>109.71</v>
-      </c>
-      <c r="H84" s="2" t="n"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B85" s="3" t="inlineStr">
-        <is>
-          <t>08/01/2025</t>
-        </is>
-      </c>
-      <c r="C85" s="3" t="inlineStr">
-        <is>
-          <t>30/01/2025</t>
-        </is>
-      </c>
-      <c r="D85" s="3" t="n">
-        <v>22</v>
-      </c>
-      <c r="E85" s="3" t="n">
-        <v>-24.43</v>
-      </c>
-      <c r="F85" s="3" t="inlineStr">
-        <is>
-          <t>14/58</t>
-        </is>
-      </c>
-      <c r="G85" s="3" t="n">
-        <v>85.27</v>
-      </c>
-      <c r="H85" s="3" t="n"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B86" s="2" t="inlineStr">
-        <is>
-          <t>30/01/2025</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="inlineStr">
-        <is>
-          <t>05/02/2025</t>
-        </is>
-      </c>
-      <c r="D86" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E86" s="2" t="n">
-        <v>23.02</v>
-      </c>
-      <c r="F86" s="2" t="inlineStr">
-        <is>
-          <t>14/58</t>
-        </is>
-      </c>
-      <c r="G86" s="2" t="n">
-        <v>108.3</v>
-      </c>
-      <c r="H86" s="2" t="n"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B87" s="3" t="inlineStr">
-        <is>
-          <t>05/02/2025</t>
-        </is>
-      </c>
-      <c r="C87" s="3" t="inlineStr">
-        <is>
-          <t>26/02/2025</t>
-        </is>
-      </c>
-      <c r="D87" s="3" t="n">
-        <v>21</v>
-      </c>
-      <c r="E87" s="3" t="n">
-        <v>-6.43</v>
-      </c>
-      <c r="F87" s="3" t="inlineStr">
-        <is>
-          <t>46/58</t>
-        </is>
-      </c>
-      <c r="G87" s="3" t="n">
-        <v>101.86</v>
-      </c>
-      <c r="H87" s="3" t="n"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B88" s="2" t="inlineStr">
-        <is>
-          <t>26/02/2025</t>
-        </is>
-      </c>
-      <c r="C88" s="2" t="inlineStr">
-        <is>
-          <t>28/02/2025</t>
-        </is>
-      </c>
-      <c r="D88" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E88" s="2" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="F88" s="2" t="inlineStr">
-        <is>
-          <t>53/58</t>
-        </is>
-      </c>
-      <c r="G88" s="2" t="n">
-        <v>104.35</v>
-      </c>
-      <c r="H88" s="2" t="n"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B89" s="3" t="inlineStr">
-        <is>
-          <t>28/02/2025</t>
-        </is>
-      </c>
-      <c r="C89" s="3" t="inlineStr">
-        <is>
-          <t>01/04/2025</t>
-        </is>
-      </c>
-      <c r="D89" s="3" t="n">
-        <v>31</v>
-      </c>
-      <c r="E89" s="3" t="n">
-        <v>-18.79</v>
-      </c>
-      <c r="F89" s="3" t="inlineStr">
-        <is>
-          <t>22/58</t>
-        </is>
-      </c>
-      <c r="G89" s="3" t="n">
-        <v>85.56</v>
-      </c>
-      <c r="H89" s="3" t="n"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B90" s="2" t="inlineStr">
-        <is>
-          <t>01/04/2025</t>
-        </is>
-      </c>
-      <c r="C90" s="2" t="inlineStr">
-        <is>
-          <t>03/04/2025</t>
-        </is>
-      </c>
-      <c r="D90" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E90" s="2" t="n">
-        <v>3.73</v>
-      </c>
-      <c r="F90" s="2" t="inlineStr">
-        <is>
-          <t>50/58</t>
-        </is>
-      </c>
-      <c r="G90" s="2" t="n">
-        <v>89.29000000000001</v>
-      </c>
-      <c r="H90" s="2" t="n"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B91" s="3" t="inlineStr">
-        <is>
-          <t>03/04/2025</t>
-        </is>
-      </c>
-      <c r="C91" s="3" t="inlineStr">
-        <is>
-          <t>11/04/2025</t>
-        </is>
-      </c>
-      <c r="D91" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="E91" s="3" t="n">
-        <v>-24.46</v>
-      </c>
-      <c r="F91" s="3" t="inlineStr">
-        <is>
-          <t>13/58</t>
-        </is>
-      </c>
-      <c r="G91" s="3" t="n">
-        <v>64.83</v>
-      </c>
-      <c r="H91" s="3" t="n"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B92" s="2" t="inlineStr">
-        <is>
-          <t>11/04/2025</t>
-        </is>
-      </c>
-      <c r="C92" s="2" t="inlineStr">
-        <is>
-          <t>15/04/2025</t>
-        </is>
-      </c>
-      <c r="D92" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <v>6.67</v>
-      </c>
-      <c r="F92" s="2" t="inlineStr">
-        <is>
-          <t>44/58</t>
-        </is>
-      </c>
-      <c r="G92" s="2" t="n">
-        <v>71.5</v>
-      </c>
-      <c r="H92" s="2" t="n"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B93" s="3" t="inlineStr">
-        <is>
-          <t>15/04/2025</t>
-        </is>
-      </c>
-      <c r="C93" s="3" t="inlineStr">
-        <is>
-          <t>22/04/2025</t>
-        </is>
-      </c>
-      <c r="D93" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="E93" s="3" t="n">
-        <v>-6.25</v>
-      </c>
-      <c r="F93" s="3" t="inlineStr">
-        <is>
-          <t>47/58</t>
-        </is>
-      </c>
-      <c r="G93" s="3" t="n">
-        <v>65.25</v>
-      </c>
-      <c r="H93" s="3" t="n"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B94" s="2" t="inlineStr">
-        <is>
-          <t>22/04/2025</t>
-        </is>
-      </c>
-      <c r="C94" s="2" t="inlineStr">
-        <is>
-          <t>29/04/2025</t>
-        </is>
-      </c>
-      <c r="D94" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <v>8.57</v>
-      </c>
-      <c r="F94" s="2" t="inlineStr">
-        <is>
-          <t>37/58</t>
-        </is>
-      </c>
-      <c r="G94" s="2" t="n">
-        <v>73.81999999999999</v>
-      </c>
-      <c r="H94" s="2" t="n"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B95" s="3" t="inlineStr">
-        <is>
-          <t>29/04/2025</t>
-        </is>
-      </c>
-      <c r="C95" s="3" t="inlineStr">
-        <is>
-          <t>06/05/2025</t>
-        </is>
-      </c>
-      <c r="D95" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="E95" s="3" t="n">
-        <v>-5.26</v>
-      </c>
-      <c r="F95" s="3" t="inlineStr">
-        <is>
-          <t>48/58</t>
-        </is>
-      </c>
-      <c r="G95" s="3" t="n">
-        <v>68.56</v>
-      </c>
-      <c r="H95" s="3" t="n"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B96" s="2" t="inlineStr">
-        <is>
-          <t>06/05/2025</t>
-        </is>
-      </c>
-      <c r="C96" s="2" t="inlineStr">
-        <is>
-          <t>12/05/2025</t>
-        </is>
-      </c>
-      <c r="D96" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E96" s="2" t="n">
-        <v>12.96</v>
-      </c>
-      <c r="F96" s="2" t="inlineStr">
-        <is>
-          <t>27/58</t>
-        </is>
-      </c>
-      <c r="G96" s="2" t="n">
-        <v>81.52</v>
-      </c>
-      <c r="H96" s="2" t="n"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B97" s="3" t="inlineStr">
-        <is>
-          <t>12/05/2025</t>
-        </is>
-      </c>
-      <c r="C97" s="3" t="inlineStr">
-        <is>
-          <t>19/05/2025</t>
-        </is>
-      </c>
-      <c r="D97" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="E97" s="3" t="n">
-        <v>-9.84</v>
-      </c>
-      <c r="F97" s="3" t="inlineStr">
-        <is>
-          <t>39/58</t>
-        </is>
-      </c>
-      <c r="G97" s="3" t="n">
-        <v>71.68000000000001</v>
-      </c>
-      <c r="H97" s="3" t="n"/>
-    </row>
-    <row r="98">
-      <c r="A98" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B98" s="2" t="inlineStr">
-        <is>
-          <t>19/05/2025</t>
-        </is>
-      </c>
-      <c r="C98" s="2" t="inlineStr">
-        <is>
-          <t>27/05/2025</t>
-        </is>
-      </c>
-      <c r="D98" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E98" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="F98" s="2" t="inlineStr">
-        <is>
-          <t>11/58</t>
-        </is>
-      </c>
-      <c r="G98" s="2" t="n">
-        <v>101.68</v>
-      </c>
-      <c r="H98" s="2" t="inlineStr">
-        <is>
-          <t>23/05/2025, 27/05/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B99" s="3" t="inlineStr">
-        <is>
-          <t>27/05/2025</t>
-        </is>
-      </c>
-      <c r="C99" s="3" t="inlineStr">
-        <is>
-          <t>12/06/2025</t>
-        </is>
-      </c>
-      <c r="D99" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="E99" s="3" t="n">
-        <v>-21.68</v>
-      </c>
-      <c r="F99" s="3" t="inlineStr">
-        <is>
-          <t>18/58</t>
-        </is>
-      </c>
-      <c r="G99" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="H99" s="3" t="inlineStr">
-        <is>
-          <t>02/06/2025, 06/06/2025, 09/06/2025, 10/06/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B100" s="2" t="inlineStr">
-        <is>
-          <t>12/06/2025</t>
-        </is>
-      </c>
-      <c r="C100" s="2" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="D100" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E100" s="2" t="n">
-        <v>4.46</v>
-      </c>
-      <c r="F100" s="2" t="inlineStr">
-        <is>
-          <t>48/58</t>
-        </is>
-      </c>
-      <c r="G100" s="2" t="n">
-        <v>84.47</v>
-      </c>
-      <c r="H100" s="2" t="n"/>
-    </row>
-    <row r="101">
-      <c r="A101" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B101" s="3" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C101" s="3" t="inlineStr">
-        <is>
-          <t>20/06/2025</t>
-        </is>
-      </c>
-      <c r="D101" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E101" s="3" t="n">
-        <v>-11.97</v>
-      </c>
-      <c r="F101" s="3" t="inlineStr">
-        <is>
-          <t>32/58</t>
-        </is>
-      </c>
-      <c r="G101" s="3" t="n">
-        <v>72.5</v>
-      </c>
-      <c r="H101" s="3" t="n"/>
-    </row>
-    <row r="102">
-      <c r="A102" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B102" s="2" t="inlineStr">
-        <is>
-          <t>20/06/2025</t>
-        </is>
-      </c>
-      <c r="C102" s="2" t="inlineStr">
-        <is>
-          <t>25/06/2025</t>
-        </is>
-      </c>
-      <c r="D102" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E102" s="2" t="n">
-        <v>11.65</v>
-      </c>
-      <c r="F102" s="2" t="inlineStr">
-        <is>
-          <t>29/58</t>
-        </is>
-      </c>
-      <c r="G102" s="2" t="n">
-        <v>84.15000000000001</v>
-      </c>
-      <c r="H102" s="2" t="n"/>
-    </row>
-    <row r="103">
-      <c r="A103" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B103" s="3" t="inlineStr">
-        <is>
-          <t>25/06/2025</t>
-        </is>
-      </c>
-      <c r="C103" s="3" t="inlineStr">
-        <is>
-          <t>08/07/2025</t>
-        </is>
-      </c>
-      <c r="D103" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="E103" s="3" t="n">
-        <v>-0.87</v>
-      </c>
-      <c r="F103" s="3" t="inlineStr">
-        <is>
-          <t>57/58</t>
-        </is>
-      </c>
-      <c r="G103" s="3" t="n">
-        <v>83.28</v>
-      </c>
-      <c r="H103" s="3" t="n"/>
-    </row>
-    <row r="104">
-      <c r="A104" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B104" s="2" t="inlineStr">
-        <is>
-          <t>08/07/2025</t>
-        </is>
-      </c>
-      <c r="C104" s="2" t="inlineStr">
-        <is>
-          <t>11/07/2025</t>
-        </is>
-      </c>
-      <c r="D104" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E104" s="2" t="n">
-        <v>30.77</v>
-      </c>
-      <c r="F104" s="2" t="inlineStr">
-        <is>
-          <t>10/58</t>
-        </is>
-      </c>
-      <c r="G104" s="2" t="n">
-        <v>114.05</v>
-      </c>
-      <c r="H104" s="2" t="n"/>
-    </row>
-    <row r="105">
-      <c r="A105" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B105" s="3" t="inlineStr">
-        <is>
-          <t>11/07/2025</t>
-        </is>
-      </c>
-      <c r="C105" s="3" t="inlineStr">
-        <is>
-          <t>13/08/2025</t>
-        </is>
-      </c>
-      <c r="D105" s="3" t="n">
-        <v>33</v>
-      </c>
-      <c r="E105" s="3" t="n">
-        <v>-15.69</v>
-      </c>
-      <c r="F105" s="3" t="inlineStr">
-        <is>
-          <t>25/58</t>
-        </is>
-      </c>
-      <c r="G105" s="3" t="n">
-        <v>98.37</v>
-      </c>
-      <c r="H105" s="3" t="n"/>
-    </row>
-    <row r="106">
-      <c r="A106" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B106" s="2" t="inlineStr">
-        <is>
-          <t>13/08/2025</t>
-        </is>
-      </c>
-      <c r="C106" s="2" t="inlineStr">
-        <is>
-          <t>15/08/2025</t>
-        </is>
-      </c>
-      <c r="D106" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E106" s="2" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="F106" s="2" t="inlineStr">
-        <is>
-          <t>43/58</t>
-        </is>
-      </c>
-      <c r="G106" s="2" t="n">
-        <v>105.17</v>
-      </c>
-      <c r="H106" s="2" t="n"/>
-    </row>
-    <row r="107">
-      <c r="A107" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B107" s="3" t="inlineStr">
-        <is>
-          <t>15/08/2025</t>
-        </is>
-      </c>
-      <c r="C107" s="3" t="inlineStr">
-        <is>
-          <t>21/08/2025</t>
-        </is>
-      </c>
-      <c r="D107" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E107" s="3" t="n">
-        <v>-7.64</v>
-      </c>
-      <c r="F107" s="3" t="inlineStr">
-        <is>
-          <t>44/58</t>
-        </is>
-      </c>
-      <c r="G107" s="3" t="n">
-        <v>97.53</v>
-      </c>
-      <c r="H107" s="3" t="n"/>
-    </row>
-    <row r="108">
-      <c r="A108" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B108" s="2" t="inlineStr">
-        <is>
-          <t>21/08/2025</t>
-        </is>
-      </c>
-      <c r="C108" s="2" t="inlineStr">
-        <is>
-          <t>28/08/2025</t>
-        </is>
-      </c>
-      <c r="D108" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E108" s="2" t="n">
-        <v>7.59</v>
-      </c>
-      <c r="F108" s="2" t="inlineStr">
-        <is>
-          <t>40/58</t>
-        </is>
-      </c>
-      <c r="G108" s="2" t="n">
-        <v>105.11</v>
-      </c>
-      <c r="H108" s="2" t="n"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B109" s="3" t="inlineStr">
-        <is>
-          <t>28/08/2025</t>
-        </is>
-      </c>
-      <c r="C109" s="3" t="inlineStr">
-        <is>
-          <t>29/09/2025</t>
-        </is>
-      </c>
-      <c r="D109" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="E109" s="3" t="n">
-        <v>-5.13</v>
-      </c>
-      <c r="F109" s="3" t="inlineStr">
-        <is>
-          <t>49/58</t>
-        </is>
-      </c>
-      <c r="G109" s="3" t="n">
-        <v>99.98</v>
-      </c>
-      <c r="H109" s="3" t="n"/>
-    </row>
-    <row r="110">
-      <c r="A110" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B110" s="2" t="inlineStr">
-        <is>
-          <t>29/09/2025</t>
-        </is>
-      </c>
-      <c r="C110" s="2" t="inlineStr">
-        <is>
-          <t>06/10/2025</t>
-        </is>
-      </c>
-      <c r="D110" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E110" s="2" t="n">
-        <v>3.38</v>
-      </c>
-      <c r="F110" s="2" t="inlineStr">
-        <is>
-          <t>51/58</t>
-        </is>
-      </c>
-      <c r="G110" s="2" t="n">
-        <v>103.36</v>
-      </c>
-      <c r="H110" s="2" t="n"/>
-    </row>
-    <row r="111">
-      <c r="A111" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B111" s="3" t="inlineStr">
-        <is>
-          <t>06/10/2025</t>
-        </is>
-      </c>
-      <c r="C111" s="3" t="inlineStr">
-        <is>
-          <t>29/10/2025</t>
-        </is>
-      </c>
-      <c r="D111" s="3" t="n">
-        <v>23</v>
-      </c>
-      <c r="E111" s="3" t="n">
-        <v>-19.61</v>
-      </c>
-      <c r="F111" s="3" t="inlineStr">
-        <is>
-          <t>20/58</t>
-        </is>
-      </c>
-      <c r="G111" s="3" t="n">
-        <v>83.75</v>
-      </c>
-      <c r="H111" s="3" t="n"/>
-    </row>
-    <row r="112">
-      <c r="A112" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B112" s="2" t="inlineStr">
-        <is>
-          <t>29/10/2025</t>
-        </is>
-      </c>
-      <c r="C112" s="2" t="inlineStr">
-        <is>
-          <t>14/11/2025</t>
-        </is>
-      </c>
-      <c r="D112" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="E112" s="2" t="n">
-        <v>11.36</v>
-      </c>
-      <c r="F112" s="2" t="inlineStr">
-        <is>
-          <t>31/58</t>
-        </is>
-      </c>
-      <c r="G112" s="2" t="n">
-        <v>95.12</v>
-      </c>
-      <c r="H112" s="2" t="n"/>
-    </row>
-    <row r="113">
-      <c r="A113" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B113" s="3" t="inlineStr">
-        <is>
-          <t>14/11/2025</t>
-        </is>
-      </c>
-      <c r="C113" s="3" t="inlineStr">
-        <is>
-          <t>08/12/2025</t>
-        </is>
-      </c>
-      <c r="D113" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E113" s="3" t="n">
-        <v>-16.33</v>
-      </c>
-      <c r="F113" s="3" t="inlineStr">
-        <is>
-          <t>24/58</t>
-        </is>
-      </c>
-      <c r="G113" s="3" t="n">
-        <v>78.79000000000001</v>
-      </c>
-      <c r="H113" s="3" t="n"/>
-    </row>
-    <row r="114">
-      <c r="A114" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B114" s="2" t="inlineStr">
-        <is>
-          <t>08/12/2025</t>
-        </is>
-      </c>
-      <c r="C114" s="2" t="inlineStr">
-        <is>
-          <t>11/12/2025</t>
-        </is>
-      </c>
-      <c r="D114" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E114" s="2" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="F114" s="2" t="inlineStr">
-        <is>
-          <t>41/58</t>
-        </is>
-      </c>
-      <c r="G114" s="2" t="n">
-        <v>86.11</v>
-      </c>
-      <c r="H114" s="2" t="n"/>
-    </row>
-    <row r="115">
-      <c r="A115" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B115" s="3" t="inlineStr">
-        <is>
-          <t>11/12/2025</t>
-        </is>
-      </c>
-      <c r="C115" s="3" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
-      <c r="D115" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E115" s="3" t="n">
-        <v>-16.67</v>
-      </c>
-      <c r="F115" s="3" t="inlineStr">
-        <is>
-          <t>23/58</t>
-        </is>
-      </c>
-      <c r="G115" s="3" t="n">
-        <v>69.44</v>
-      </c>
-      <c r="H115" s="3" t="n"/>
-    </row>
-    <row r="116">
-      <c r="A116" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B116" s="2" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
-      <c r="C116" s="2" t="inlineStr">
-        <is>
-          <t>03/02/2026</t>
-        </is>
-      </c>
-      <c r="D116" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="E116" s="2" t="n">
-        <v>39.09</v>
-      </c>
-      <c r="F116" s="2" t="inlineStr">
-        <is>
-          <t>7/58</t>
-        </is>
-      </c>
-      <c r="G116" s="2" t="n">
-        <v>108.53</v>
-      </c>
-      <c r="H116" s="2" t="n"/>
-    </row>
-    <row r="117">
-      <c r="A117" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B117" s="3" t="inlineStr">
-        <is>
-          <t>03/02/2026</t>
-        </is>
-      </c>
-      <c r="C117" s="3" t="inlineStr">
-        <is>
-          <t>11/02/2026</t>
-        </is>
-      </c>
-      <c r="D117" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="E117" s="3" t="n">
-        <v>-3.27</v>
-      </c>
-      <c r="F117" s="3" t="inlineStr">
-        <is>
-          <t>52/58</t>
-        </is>
-      </c>
-      <c r="G117" s="3" t="n">
-        <v>105.26</v>
-      </c>
-      <c r="H117" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update absorption event logic; refine buy order tracking
Enhanced the absorption event handling and buy order tracking in the insider conviction strategy. Updated related output files and UI components to reflect the changes.

- Updated `grov_insider_conviction_poc.json` with new trade data and metrics
- Modified `grov_rise_events.xlsx` to include updated event details
- Refined logic in `backtest_insider_conviction_strategy.py` for absorption events
- Adjusted `AllChartsView.jsx` to display updated data
- Added temporary file `~$grov_rise_events.xlsx` for intermediate processing

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/grov_rise_events.xlsx
+++ b/output CSVs/grov_rise_events.xlsx
@@ -691,11 +691,7 @@
       <c r="G7" s="3" t="n">
         <v>-28.62</v>
       </c>
-      <c r="H7" s="3" t="inlineStr">
-        <is>
-          <t>30/08/2022</t>
-        </is>
-      </c>
+      <c r="H7" s="3" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -1281,7 +1277,7 @@
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>17/05/2023, 22/05/2023, 23/05/2023, 24/05/2023, 26/05/2023, 30/05/2023, 01/06/2023</t>
+          <t>17/05/2023</t>
         </is>
       </c>
     </row>
@@ -2777,7 +2773,7 @@
       </c>
       <c r="H71" s="3" t="inlineStr">
         <is>
-          <t>02/06/2025, 06/06/2025, 09/06/2025, 10/06/2025, 12/06/2025, 13/06/2025</t>
+          <t>02/06/2025, 09/06/2025, 10/06/2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add JSON generation for mid rises and falls in script output
Updated the script and related files to include JSON generation for mid rises and falls. Adjusted data structures and output formats to align with the new functionality.

- Modified `backtest_insider_conviction_strategy.py` to generate JSON for mid rises and falls
- Updated `grov_insider_conviction_poc.json` with revised trade data and structure
- Adjusted `grov_rise_events.xlsx` and `grov_rise_volatility_analysis.json` for consistency
- Updated `AllChartsView.jsx` to support new JSON data visualization
- Refined data handling and output logic in the script for better accuracy and performance

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/grov_rise_events.xlsx
+++ b/output CSVs/grov_rise_events.xlsx
@@ -691,7 +691,11 @@
       <c r="G7" s="3" t="n">
         <v>-28.62</v>
       </c>
-      <c r="H7" s="3" t="n"/>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>30/08/2022</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -1277,7 +1281,7 @@
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>17/05/2023</t>
+          <t>17/05/2023, 22/05/2023, 23/05/2023, 24/05/2023, 26/05/2023, 30/05/2023, 01/06/2023</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2777,7 @@
       </c>
       <c r="H71" s="3" t="inlineStr">
         <is>
-          <t>02/06/2025, 09/06/2025, 10/06/2025</t>
+          <t>02/06/2025, 06/06/2025, 09/06/2025, 10/06/2025, 12/06/2025, 13/06/2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enable big test execution for single stock analysis
Enhanced scripts and outputs to support focused testing on individual stocks. Adjusted insider conviction strategy data and added new outputs for rise events and volatility analysis.

- Updated `.github/copilot-instructions.md` with critical trading strategy rules.
- Modified insider conviction strategy scripts for single stock testing.
- Adjusted GROV insider conviction POC data for improved accuracy.
- Added new outputs for BSFC rise events and volatility analysis.
- Removed outdated GROV rise events temporary file.
- Updated PID files for node-server and Vite processes.

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/grov_rise_events.xlsx
+++ b/output CSVs/grov_rise_events.xlsx
@@ -1085,7 +1085,7 @@
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>17/03/2023</t>
+          <t>17/03/2023, 20/03/2023</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>17/05/2023, 22/05/2023, 23/05/2023, 24/05/2023, 26/05/2023, 30/05/2023, 01/06/2023</t>
+          <t>17/05/2023, 22/05/2023, 23/05/2023, 24/05/2023, 26/05/2023, 30/05/2023, 01/06/2023, 09/06/2023</t>
         </is>
       </c>
     </row>

</xml_diff>